<commit_message>
chassis params extraction function add
</commit_message>
<xml_diff>
--- a/san_automation_info.xlsx
+++ b/san_automation_info.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <fileSharing readOnlyRecommended="0" userName="kvl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlasenko\Documents\05.PYTHON\Projects\san_report_automation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="3" xWindow="240" yWindow="60" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="switch_info" sheetId="1" r:id="rId4"/>
-    <sheet name="parameters" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
-    <sheet name="columns" sheetId="4" r:id="rId7"/>
+    <sheet name="switch_info" sheetId="1" r:id="rId1"/>
+    <sheet name="parameters" sheetId="2" r:id="rId2"/>
+    <sheet name="columns" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr iterateDelta="0.0001"/>
+  <calcPr calcId="4283453520" iterateDelta="1E-4"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:revision xmlns:pm="smNativeData" day="1564686220" val="966" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="424">
   <si>
     <t>switchType</t>
   </si>
@@ -1274,70 +1278,49 @@
   </si>
   <si>
     <t>Number_of_LS</t>
+  </si>
+  <si>
+    <t>ts.tz</t>
+  </si>
+  <si>
+    <t>snmp_server</t>
+  </si>
+  <si>
+    <t>syslog_server</t>
+  </si>
+  <si>
+    <t>timezone_h:m</t>
+  </si>
+  <si>
+    <t>chassis_wwn</t>
+  </si>
+  <si>
+    <t>config_collection_date</t>
+  </si>
+  <si>
+    <t>chassis_params_add</t>
+  </si>
+  <si>
+    <t>timezone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="10">
-    <numFmt numFmtId="5" formatCode="#,##0\ &quot;₽&quot;;\-#,##0\ &quot;₽&quot;"/>
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;₽&quot;;[Red]\-#,##0\ &quot;₽&quot;"/>
-    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;₽&quot;;\-#,##0.00\ &quot;₽&quot;"/>
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;₽&quot;;[Red]\-#,##0.00\ &quot;₽&quot;"/>
-    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₽&quot;_-;\-* #,##0\ &quot;₽&quot;_-;_-* &quot;-&quot;\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0\ _₽_-;\-* #,##0\ _₽_-;_-* &quot;-&quot;\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="2" formatCode="0.00"/>
-    <numFmt numFmtId="49" formatCode="@"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1564686220" ulstyle="none" kern="1">
-            <pm:latin face="Calibri" sz="220" lang="default"/>
-            <pm:cs face="Basic Roman" sz="220" lang="default"/>
-            <pm:ea face="Basic Roman" sz="220" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
     </font>
     <font>
-      <name val="Basic Sans"/>
-      <family val="1"/>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1564686220" ulstyle="none" kern="1">
-            <pm:latin face="Basic Sans" sz="200" lang="default"/>
-            <pm:cs face="Basic Roman" sz="200" lang="default"/>
-            <pm:ea face="Basic Roman" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <b/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1564686220" ulstyle="none" kern="1">
-            <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
-            <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
-            <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
     </font>
   </fonts>
   <fills count="3">
@@ -1349,79 +1332,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1564686220" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1564686220"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1564686220"/>
-        </ext>
-      </extLst>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
     <ext uri="smNativeData">
       <pm:charStyles xmlns:pm="smNativeData" id="1564686220" count="1">
         <pm:charStyle name="Обычный" fontId="0" Id="1"/>
@@ -1686,24 +1644,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.40"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.571429" customWidth="1" style="1"/>
-    <col min="2" max="2" width="57.428571" customWidth="1"/>
-    <col min="3" max="3" width="58.714286" customWidth="1"/>
-    <col min="4" max="4" width="30.857143" customWidth="1"/>
-    <col min="5" max="5" width="58.714286" customWidth="1"/>
-    <col min="6" max="1025" width="8.571429" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
+    <col min="3" max="3" width="58.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="5" max="5" width="58.7109375" customWidth="1"/>
+    <col min="6" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1720,8 +1678,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1737,8 +1695,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1754,8 +1712,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1771,8 +1729,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1788,8 +1746,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -1805,8 +1763,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -1822,8 +1780,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -1839,8 +1797,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>9</v>
       </c>
       <c r="B9" t="s">
@@ -1856,8 +1814,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>10</v>
       </c>
       <c r="B10" t="s">
@@ -1873,8 +1831,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>12</v>
       </c>
       <c r="B11" t="s">
@@ -1890,8 +1848,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>16</v>
       </c>
       <c r="B12" t="s">
@@ -1907,8 +1865,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>17</v>
       </c>
       <c r="B13" t="s">
@@ -1924,8 +1882,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>18</v>
       </c>
       <c r="B14" t="s">
@@ -1941,8 +1899,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>21</v>
       </c>
       <c r="B15" t="s">
@@ -1958,8 +1916,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>22</v>
       </c>
       <c r="B16" t="s">
@@ -1975,8 +1933,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>26</v>
       </c>
       <c r="B17" t="s">
@@ -1992,8 +1950,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>27</v>
       </c>
       <c r="B18" t="s">
@@ -2009,8 +1967,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>29</v>
       </c>
       <c r="B19" t="s">
@@ -2026,8 +1984,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>32</v>
       </c>
       <c r="B20" t="s">
@@ -2043,8 +2001,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>33</v>
       </c>
       <c r="B21" t="s">
@@ -2060,8 +2018,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>34</v>
       </c>
       <c r="B22" t="s">
@@ -2077,8 +2035,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>37</v>
       </c>
       <c r="B23" t="s">
@@ -2094,8 +2052,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>38</v>
       </c>
       <c r="B24" t="s">
@@ -2111,8 +2069,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>40</v>
       </c>
       <c r="B25" t="s">
@@ -2128,8 +2086,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>41</v>
       </c>
       <c r="B26" t="s">
@@ -2145,8 +2103,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>42</v>
       </c>
       <c r="B27" t="s">
@@ -2162,8 +2120,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1" t="n">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>43</v>
       </c>
       <c r="B28" t="s">
@@ -2179,8 +2137,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1" t="n">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>44</v>
       </c>
       <c r="B29" t="s">
@@ -2196,8 +2154,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="1" t="n">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>45</v>
       </c>
       <c r="B30" t="s">
@@ -2213,8 +2171,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="1" t="n">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>46</v>
       </c>
       <c r="B31" t="s">
@@ -2227,8 +2185,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="1" t="n">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>51</v>
       </c>
       <c r="B32" t="s">
@@ -2244,9 +2202,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1" t="n">
-        <v>55.2000000000000028</v>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>55.2</v>
       </c>
       <c r="B33" t="s">
         <v>41</v>
@@ -2261,8 +2219,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1" t="n">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>58</v>
       </c>
       <c r="B34" t="s">
@@ -2278,8 +2236,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1" t="n">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>61</v>
       </c>
       <c r="B35" t="s">
@@ -2295,8 +2253,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="1" t="n">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>62</v>
       </c>
       <c r="B36" t="s">
@@ -2312,8 +2270,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1" t="n">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>64</v>
       </c>
       <c r="B37" t="s">
@@ -2329,8 +2287,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1" t="n">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>66</v>
       </c>
       <c r="B38" t="s">
@@ -2346,8 +2304,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="1" t="n">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>67</v>
       </c>
       <c r="B39" t="s">
@@ -2363,8 +2321,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="1" t="n">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>69</v>
       </c>
       <c r="B40" t="s">
@@ -2380,8 +2338,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="1" t="n">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>70</v>
       </c>
       <c r="B41" t="s">
@@ -2397,8 +2355,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="1" t="n">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>71</v>
       </c>
       <c r="B42" t="s">
@@ -2411,8 +2369,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="1" t="n">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>72</v>
       </c>
       <c r="B43" t="s">
@@ -2428,8 +2386,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="1" t="n">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>73</v>
       </c>
       <c r="B44" t="s">
@@ -2445,8 +2403,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="1" t="n">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>75</v>
       </c>
       <c r="B45" t="s">
@@ -2462,8 +2420,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="1" t="n">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>76</v>
       </c>
       <c r="B46" t="s">
@@ -2479,8 +2437,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="1" t="n">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>77</v>
       </c>
       <c r="B47" t="s">
@@ -2496,8 +2454,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="1" t="n">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>83</v>
       </c>
       <c r="B48" t="s">
@@ -2513,8 +2471,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="1" t="n">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>86</v>
       </c>
       <c r="B49" t="s">
@@ -2530,8 +2488,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="1" t="n">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>87</v>
       </c>
       <c r="B50" t="s">
@@ -2547,8 +2505,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="1" t="n">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>90</v>
       </c>
       <c r="B51" t="s">
@@ -2564,8 +2522,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="1" t="n">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>92</v>
       </c>
       <c r="B52" t="s">
@@ -2581,8 +2539,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="1" t="n">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
         <v>95</v>
       </c>
       <c r="B53" t="s">
@@ -2598,8 +2556,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="1" t="n">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>96</v>
       </c>
       <c r="B54" t="s">
@@ -2615,8 +2573,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="1" t="n">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>97</v>
       </c>
       <c r="B55" t="s">
@@ -2632,8 +2590,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="1" t="n">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
         <v>98</v>
       </c>
       <c r="B56" t="s">
@@ -2649,8 +2607,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="1" t="n">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>108</v>
       </c>
       <c r="B57" t="s">
@@ -2666,8 +2624,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="1" t="n">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>109</v>
       </c>
       <c r="B58" t="s">
@@ -2683,8 +2641,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="1" t="n">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>116</v>
       </c>
       <c r="B59" t="s">
@@ -2700,8 +2658,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="1" t="n">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
         <v>117</v>
       </c>
       <c r="B60" t="s">
@@ -2717,8 +2675,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="1" t="n">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>118</v>
       </c>
       <c r="B61" t="s">
@@ -2734,8 +2692,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="1" t="n">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
         <v>120</v>
       </c>
       <c r="B62" t="s">
@@ -2751,8 +2709,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="1" t="n">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
         <v>121</v>
       </c>
       <c r="B63" t="s">
@@ -2768,8 +2726,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="1" t="n">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
         <v>129</v>
       </c>
       <c r="B64" t="s">
@@ -2785,8 +2743,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="1" t="n">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
         <v>130</v>
       </c>
       <c r="B65" t="s">
@@ -2802,8 +2760,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="1" t="n">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
         <v>133</v>
       </c>
       <c r="B66" t="s">
@@ -2819,8 +2777,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="1" t="n">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
         <v>134</v>
       </c>
       <c r="B67" s="4" t="s">
@@ -2836,8 +2794,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="1" t="n">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
         <v>148</v>
       </c>
       <c r="B68" s="4" t="s">
@@ -2853,8 +2811,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="1" t="n">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
         <v>162</v>
       </c>
       <c r="B69" t="s">
@@ -2870,8 +2828,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="1" t="n">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
         <v>165</v>
       </c>
       <c r="B70" t="s">
@@ -2887,8 +2845,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="1" t="n">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
         <v>166</v>
       </c>
       <c r="B71" t="s">
@@ -2904,8 +2862,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="1" t="n">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
         <v>170</v>
       </c>
       <c r="B72" t="s">
@@ -2922,23 +2880,8 @@
       </c>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1564686220" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1564686220" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1564686220" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.51180599999999998"/>
+  <pageSetup paperSize="9" fitToWidth="0"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:sheetPrefs xmlns:pm="smNativeData" day="1564686220" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
@@ -2951,214 +2894,174 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.40"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.303571" customWidth="1"/>
-    <col min="2" max="2" width="37.732143" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B1"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>126</v>
       </c>
-      <c r="B2"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B3"/>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5"/>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>130</v>
       </c>
-      <c r="B6"/>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B7"/>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="5" t="s">
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B8"/>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10"/>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B13"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B14"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B17"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B18"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B19"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B20"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B21"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>146</v>
-      </c>
-      <c r="B22"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>147</v>
-      </c>
-      <c r="B23"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B24"/>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="5"/>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="7" t="s">
-        <v>154</v>
-      </c>
+      <c r="B20" s="5"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1564686220" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.300000" footer="0.300000"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1564686220" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1564686220" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" fitToWidth="0" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:sheetPrefs xmlns:pm="smNativeData" day="1564686220" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
@@ -3171,1293 +3074,203 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.40"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.857143" customWidth="1" style="5"/>
-    <col min="2" max="2" width="44.857143" customWidth="1" style="5"/>
-    <col min="3" max="3" width="45.285714" customWidth="1" style="5"/>
-    <col min="4" max="4" width="32.714286" customWidth="1"/>
-    <col min="5" max="5" width="36.428571" customWidth="1"/>
-    <col min="6" max="6" width="33.428571" customWidth="1"/>
-    <col min="7" max="7" width="28.000000" customWidth="1"/>
-    <col min="8" max="9" width="24.714286" customWidth="1"/>
-    <col min="10" max="10" width="26.571429" customWidth="1"/>
-    <col min="11" max="11" width="20.285714" customWidth="1"/>
-    <col min="12" max="12" width="22.000000" customWidth="1"/>
-    <col min="13" max="13" width="21.571429" customWidth="1"/>
-    <col min="14" max="14" width="8.571429" customWidth="1"/>
-    <col min="15" max="15" width="21.000000" customWidth="1"/>
-    <col min="16" max="1025" width="8.571429" customWidth="1"/>
+    <col min="1" max="1" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G2" s="5" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="I2" t="s">
-        <v>173</v>
-      </c>
-      <c r="J2" t="s">
-        <v>174</v>
-      </c>
-      <c r="K2" t="s">
-        <v>172</v>
-      </c>
-      <c r="L2" t="s">
-        <v>175</v>
-      </c>
-      <c r="M2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="5" t="s">
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="F3" t="s">
-        <v>178</v>
-      </c>
-      <c r="G3" t="s">
-        <v>168</v>
-      </c>
-      <c r="H3" t="s">
-        <v>179</v>
-      </c>
-      <c r="I3" t="s">
-        <v>180</v>
-      </c>
-      <c r="J3" t="s">
-        <v>181</v>
-      </c>
-      <c r="K3" t="s">
-        <v>168</v>
-      </c>
-      <c r="L3" t="s">
-        <v>182</v>
-      </c>
-      <c r="M3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="G4" t="s">
-        <v>186</v>
-      </c>
-      <c r="H4" t="s">
-        <v>187</v>
-      </c>
-      <c r="I4" t="s">
-        <v>188</v>
-      </c>
-      <c r="J4" t="s">
-        <v>189</v>
-      </c>
-      <c r="K4" t="s">
-        <v>190</v>
-      </c>
-      <c r="L4" t="s">
-        <v>191</v>
-      </c>
-      <c r="M4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B7" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="F5" t="s">
-        <v>195</v>
-      </c>
-      <c r="G5" t="s">
-        <v>190</v>
-      </c>
-      <c r="H5" t="s">
-        <v>196</v>
-      </c>
-      <c r="I5" t="s">
-        <v>197</v>
-      </c>
-      <c r="J5" t="s">
-        <v>198</v>
-      </c>
-      <c r="K5" t="s">
-        <v>199</v>
-      </c>
-      <c r="L5" t="s">
-        <v>192</v>
-      </c>
-      <c r="M5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="F6" t="s">
-        <v>203</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="H6" t="s">
-        <v>204</v>
-      </c>
-      <c r="I6" t="s">
-        <v>205</v>
-      </c>
-      <c r="J6" t="s">
-        <v>206</v>
-      </c>
-      <c r="K6" t="s">
-        <v>207</v>
-      </c>
-      <c r="L6" t="s">
-        <v>208</v>
-      </c>
-      <c r="M6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G7" t="s">
-        <v>212</v>
-      </c>
-      <c r="H7" t="s">
-        <v>213</v>
-      </c>
-      <c r="I7" t="s">
-        <v>214</v>
-      </c>
-      <c r="J7" t="s">
-        <v>215</v>
-      </c>
-      <c r="K7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L7" t="s">
-        <v>217</v>
-      </c>
-      <c r="M7" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F8" t="s">
-        <v>220</v>
-      </c>
-      <c r="G8" t="s">
-        <v>221</v>
-      </c>
-      <c r="H8" t="s">
-        <v>222</v>
-      </c>
-      <c r="I8" t="s">
-        <v>223</v>
-      </c>
-      <c r="J8" t="s">
-        <v>224</v>
-      </c>
-      <c r="K8" t="s">
-        <v>225</v>
-      </c>
-      <c r="L8" t="s">
-        <v>226</v>
-      </c>
-      <c r="M8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F9" t="s">
-        <v>229</v>
-      </c>
-      <c r="G9" t="s">
-        <v>230</v>
-      </c>
-      <c r="H9" t="s">
-        <v>231</v>
-      </c>
-      <c r="I9" t="s">
-        <v>232</v>
-      </c>
-      <c r="J9" t="s">
-        <v>233</v>
-      </c>
-      <c r="K9" t="s">
-        <v>234</v>
-      </c>
-      <c r="L9" t="s">
-        <v>235</v>
-      </c>
-      <c r="M9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F10" t="s">
-        <v>238</v>
-      </c>
-      <c r="G10" t="s">
-        <v>239</v>
-      </c>
-      <c r="H10" t="s">
-        <v>240</v>
-      </c>
-      <c r="I10" t="s">
-        <v>241</v>
-      </c>
-      <c r="J10" t="s">
-        <v>242</v>
-      </c>
-      <c r="K10" t="s">
-        <v>243</v>
-      </c>
-      <c r="L10" t="s">
-        <v>244</v>
-      </c>
-      <c r="M10" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F11" t="s">
-        <v>247</v>
-      </c>
-      <c r="G11" t="s">
-        <v>248</v>
-      </c>
-      <c r="H11" t="s">
-        <v>249</v>
-      </c>
-      <c r="I11" t="s">
-        <v>250</v>
-      </c>
-      <c r="J11" t="s">
-        <v>251</v>
-      </c>
-      <c r="K11" t="s">
-        <v>252</v>
-      </c>
-      <c r="L11" t="s">
-        <v>253</v>
-      </c>
-      <c r="M11" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F12" t="s">
-        <v>255</v>
-      </c>
-      <c r="G12" t="s">
-        <v>256</v>
-      </c>
-      <c r="I12" t="s">
-        <v>257</v>
-      </c>
-      <c r="J12" t="s">
-        <v>258</v>
-      </c>
-      <c r="K12" t="s">
-        <v>259</v>
-      </c>
-      <c r="M12" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="F13" t="s">
-        <v>262</v>
-      </c>
-      <c r="G13" t="s">
-        <v>263</v>
-      </c>
-      <c r="I13" t="s">
-        <v>264</v>
-      </c>
-      <c r="J13" t="s">
-        <v>265</v>
-      </c>
-      <c r="K13" t="s">
-        <v>266</v>
-      </c>
-      <c r="M13" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="F14" t="s">
-        <v>269</v>
-      </c>
-      <c r="G14" t="s">
-        <v>270</v>
-      </c>
-      <c r="I14" t="s">
-        <v>271</v>
-      </c>
-      <c r="J14" t="s">
-        <v>272</v>
-      </c>
-      <c r="K14" t="s">
-        <v>273</v>
-      </c>
-      <c r="M14" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F15" t="s">
-        <v>275</v>
-      </c>
-      <c r="G15" t="s">
-        <v>276</v>
-      </c>
-      <c r="I15" t="s">
-        <v>277</v>
-      </c>
-      <c r="J15" t="s">
-        <v>278</v>
-      </c>
-      <c r="K15" t="s">
-        <v>279</v>
-      </c>
-      <c r="M15" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" s="5" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F16" t="s">
-        <v>281</v>
-      </c>
-      <c r="I16" t="s">
-        <v>282</v>
-      </c>
-      <c r="J16" t="s">
-        <v>283</v>
-      </c>
-      <c r="K16" t="s">
-        <v>284</v>
-      </c>
-      <c r="M16" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="C17" s="5" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="F17" t="s">
-        <v>286</v>
-      </c>
-      <c r="I17" t="s">
-        <v>287</v>
-      </c>
-      <c r="J17" t="s">
-        <v>288</v>
-      </c>
-      <c r="K17" t="s">
-        <v>289</v>
-      </c>
-      <c r="M17" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="C18" s="5" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="F18" t="s">
-        <v>291</v>
-      </c>
-      <c r="I18" t="s">
-        <v>292</v>
-      </c>
-      <c r="J18" t="s">
-        <v>293</v>
-      </c>
-      <c r="K18" t="s">
-        <v>294</v>
-      </c>
-      <c r="M18" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F19" t="s">
-        <v>296</v>
-      </c>
-      <c r="I19" t="s">
-        <v>297</v>
-      </c>
-      <c r="J19" t="s">
-        <v>298</v>
-      </c>
-      <c r="K19" t="s">
-        <v>299</v>
-      </c>
-      <c r="M19" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F20" t="s">
-        <v>301</v>
-      </c>
-      <c r="I20" t="s">
-        <v>302</v>
-      </c>
-      <c r="J20" t="s">
-        <v>303</v>
-      </c>
-      <c r="K20" t="s">
-        <v>304</v>
-      </c>
-      <c r="M20" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="F21" t="s">
-        <v>306</v>
-      </c>
-      <c r="I21" t="s">
-        <v>307</v>
-      </c>
-      <c r="J21" t="s">
-        <v>308</v>
-      </c>
-      <c r="K21" t="s">
-        <v>309</v>
-      </c>
-      <c r="M21" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="F22" t="s">
-        <v>312</v>
-      </c>
-      <c r="I22" t="s">
-        <v>313</v>
-      </c>
-      <c r="K22" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="F23" t="s">
-        <v>317</v>
-      </c>
-      <c r="I23" t="s">
-        <v>318</v>
-      </c>
-      <c r="K23" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="F24" t="s">
-        <v>321</v>
-      </c>
-      <c r="I24" t="s">
-        <v>322</v>
-      </c>
-      <c r="K24" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="5" t="s">
-        <v>324</v>
-      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="F25" t="s">
-        <v>325</v>
-      </c>
-      <c r="I25" t="s">
-        <v>326</v>
-      </c>
-      <c r="K25" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="I26" t="s">
-        <v>329</v>
-      </c>
-      <c r="K26" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="I27" t="s">
-        <v>332</v>
-      </c>
-      <c r="K27" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="I28" t="s">
-        <v>334</v>
-      </c>
-      <c r="K28" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="I29" t="s">
-        <v>337</v>
-      </c>
-      <c r="K29" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="I30" t="s">
-        <v>340</v>
-      </c>
-      <c r="K30" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="I31" t="s">
-        <v>343</v>
-      </c>
-      <c r="K31" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="I32" t="s">
-        <v>346</v>
-      </c>
-      <c r="K32" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="I33" t="s">
-        <v>348</v>
-      </c>
-      <c r="K33" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="I34" t="s">
-        <v>350</v>
-      </c>
-      <c r="K34" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="I35" t="s">
-        <v>352</v>
-      </c>
-      <c r="K35" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="I36" t="s">
-        <v>354</v>
-      </c>
-      <c r="K36" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="I37" t="s">
-        <v>356</v>
-      </c>
-      <c r="K37" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="I38" t="s">
-        <v>359</v>
-      </c>
-      <c r="K38" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="I39" t="s">
-        <v>361</v>
-      </c>
-      <c r="K39" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="I40" t="s">
-        <v>363</v>
-      </c>
-      <c r="K40" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="I41" t="s">
-        <v>365</v>
-      </c>
-      <c r="K41" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="I42" t="s">
-        <v>367</v>
-      </c>
-      <c r="K42" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="I43" t="s">
-        <v>370</v>
-      </c>
-      <c r="K43" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I44" t="s">
-        <v>373</v>
-      </c>
-      <c r="K44" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="I45" t="s">
-        <v>376</v>
-      </c>
-      <c r="K45" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="I46" t="s">
-        <v>379</v>
-      </c>
-      <c r="K46" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="I47" t="s">
-        <v>381</v>
-      </c>
-      <c r="K47" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="I48" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I49" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>388</v>
-      </c>
-      <c r="I50" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="I51" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="I52" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9">
-      <c r="B53" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I53" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9">
-      <c r="B54" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="I54" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9">
-      <c r="B55" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="I55" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9">
-      <c r="B56" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="I56" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="57" spans="9:9">
-      <c r="I57" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="58" spans="9:9">
-      <c r="I58" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="59" spans="9:9">
-      <c r="I59" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="60" spans="9:9">
-      <c r="I60" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="61" spans="9:9">
-      <c r="I61" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="62" spans="9:9">
-      <c r="I62" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="63" spans="9:9">
-      <c r="I63" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="64" spans="9:9">
-      <c r="I64" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="65" spans="9:9">
-      <c r="I65" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="66" spans="9:9">
-      <c r="I66" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="67" spans="9:9">
-      <c r="I67" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="68" spans="9:9">
-      <c r="I68" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="69" spans="9:9">
-      <c r="I69" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="70" spans="9:9">
-      <c r="I70" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="71" spans="9:9">
-      <c r="I71" t="s">
-        <v>412</v>
-      </c>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1564686220" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.511806" footer="0.511806"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1564686220" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1564686220" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
-  </headerFooter>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.39374999999999999" footer="0.39374999999999999"/>
+  <pageSetup paperSize="9" fitToWidth="0" pageOrder="overThenDown"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:sheetPrefs xmlns:pm="smNativeData" day="1564686220" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
@@ -4470,156 +3283,1278 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="15.40"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.205357" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="45.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="8" max="9" width="24.7109375" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" customWidth="1"/>
+    <col min="15" max="15" width="21" customWidth="1"/>
+    <col min="16" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J2" t="s">
+        <v>174</v>
+      </c>
+      <c r="K2" t="s">
+        <v>172</v>
+      </c>
+      <c r="L2" t="s">
+        <v>175</v>
+      </c>
+      <c r="M2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>139</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J3" t="s">
+        <v>181</v>
+      </c>
+      <c r="K3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>128</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" t="s">
+        <v>186</v>
+      </c>
+      <c r="H4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I4" t="s">
+        <v>188</v>
+      </c>
+      <c r="J4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K4" t="s">
+        <v>190</v>
+      </c>
+      <c r="L4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G5" t="s">
+        <v>190</v>
+      </c>
+      <c r="H5" t="s">
+        <v>196</v>
+      </c>
+      <c r="I5" t="s">
+        <v>197</v>
+      </c>
+      <c r="J5" t="s">
+        <v>198</v>
+      </c>
+      <c r="K5" t="s">
+        <v>199</v>
+      </c>
+      <c r="L5" t="s">
+        <v>192</v>
+      </c>
+      <c r="M5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F6" t="s">
+        <v>203</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="H6" t="s">
+        <v>204</v>
+      </c>
+      <c r="I6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J6" t="s">
+        <v>206</v>
+      </c>
+      <c r="K6" t="s">
+        <v>207</v>
+      </c>
+      <c r="L6" t="s">
+        <v>208</v>
+      </c>
+      <c r="M6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
+        <v>210</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7" t="s">
+        <v>212</v>
+      </c>
+      <c r="H7" t="s">
+        <v>213</v>
+      </c>
+      <c r="I7" t="s">
+        <v>214</v>
+      </c>
+      <c r="J7" t="s">
+        <v>215</v>
+      </c>
+      <c r="K7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L7" t="s">
+        <v>217</v>
+      </c>
+      <c r="M7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+        <v>219</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" t="s">
+        <v>220</v>
+      </c>
+      <c r="G8" t="s">
+        <v>221</v>
+      </c>
+      <c r="H8" t="s">
+        <v>222</v>
+      </c>
+      <c r="I8" t="s">
+        <v>223</v>
+      </c>
+      <c r="J8" t="s">
+        <v>224</v>
+      </c>
+      <c r="K8" t="s">
+        <v>225</v>
+      </c>
+      <c r="L8" t="s">
+        <v>226</v>
+      </c>
+      <c r="M8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
+        <v>228</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" t="s">
+        <v>229</v>
+      </c>
+      <c r="G9" t="s">
+        <v>230</v>
+      </c>
+      <c r="H9" t="s">
+        <v>231</v>
+      </c>
+      <c r="I9" t="s">
+        <v>232</v>
+      </c>
+      <c r="J9" t="s">
+        <v>233</v>
+      </c>
+      <c r="K9" t="s">
+        <v>234</v>
+      </c>
+      <c r="L9" t="s">
+        <v>235</v>
+      </c>
+      <c r="M9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+        <v>237</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" t="s">
+        <v>238</v>
+      </c>
+      <c r="G10" t="s">
+        <v>239</v>
+      </c>
+      <c r="H10" t="s">
+        <v>240</v>
+      </c>
+      <c r="I10" t="s">
+        <v>241</v>
+      </c>
+      <c r="J10" t="s">
+        <v>242</v>
+      </c>
+      <c r="K10" t="s">
+        <v>243</v>
+      </c>
+      <c r="L10" t="s">
+        <v>244</v>
+      </c>
+      <c r="M10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
+        <v>246</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" t="s">
+        <v>247</v>
+      </c>
+      <c r="G11" t="s">
+        <v>248</v>
+      </c>
+      <c r="H11" t="s">
+        <v>249</v>
+      </c>
+      <c r="I11" t="s">
+        <v>250</v>
+      </c>
+      <c r="J11" t="s">
+        <v>251</v>
+      </c>
+      <c r="K11" t="s">
+        <v>252</v>
+      </c>
+      <c r="L11" t="s">
+        <v>253</v>
+      </c>
+      <c r="M11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
+        <v>127</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F12" t="s">
+        <v>255</v>
+      </c>
+      <c r="G12" t="s">
+        <v>256</v>
+      </c>
+      <c r="I12" t="s">
+        <v>257</v>
+      </c>
+      <c r="J12" t="s">
+        <v>258</v>
+      </c>
+      <c r="K12" t="s">
+        <v>259</v>
+      </c>
+      <c r="M12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
+        <v>261</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" t="s">
+        <v>262</v>
+      </c>
+      <c r="G13" t="s">
+        <v>263</v>
+      </c>
+      <c r="I13" t="s">
+        <v>264</v>
+      </c>
+      <c r="J13" t="s">
+        <v>265</v>
+      </c>
+      <c r="K13" t="s">
+        <v>266</v>
+      </c>
+      <c r="M13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
+        <v>268</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" t="s">
+        <v>269</v>
+      </c>
+      <c r="G14" t="s">
+        <v>270</v>
+      </c>
+      <c r="I14" t="s">
+        <v>271</v>
+      </c>
+      <c r="J14" t="s">
+        <v>272</v>
+      </c>
+      <c r="K14" t="s">
+        <v>273</v>
+      </c>
+      <c r="M14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="F15" t="s">
+        <v>275</v>
+      </c>
+      <c r="G15" t="s">
+        <v>276</v>
+      </c>
+      <c r="I15" t="s">
+        <v>277</v>
+      </c>
+      <c r="J15" t="s">
+        <v>278</v>
+      </c>
+      <c r="K15" t="s">
+        <v>279</v>
+      </c>
+      <c r="M15" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>141</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F16" t="s">
+        <v>281</v>
+      </c>
+      <c r="I16" t="s">
+        <v>282</v>
+      </c>
+      <c r="J16" t="s">
+        <v>283</v>
+      </c>
+      <c r="K16" t="s">
+        <v>284</v>
+      </c>
+      <c r="M16" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>169</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F17" t="s">
+        <v>286</v>
+      </c>
+      <c r="I17" t="s">
+        <v>287</v>
+      </c>
+      <c r="J17" t="s">
+        <v>288</v>
+      </c>
+      <c r="K17" t="s">
+        <v>289</v>
+      </c>
+      <c r="M17" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F18" t="s">
+        <v>291</v>
+      </c>
+      <c r="I18" t="s">
+        <v>292</v>
+      </c>
+      <c r="J18" t="s">
+        <v>293</v>
+      </c>
+      <c r="K18" t="s">
+        <v>294</v>
+      </c>
+      <c r="M18" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" t="s">
+        <v>296</v>
+      </c>
+      <c r="I19" t="s">
+        <v>297</v>
+      </c>
+      <c r="J19" t="s">
+        <v>298</v>
+      </c>
+      <c r="K19" t="s">
+        <v>299</v>
+      </c>
+      <c r="M19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F20" t="s">
+        <v>301</v>
+      </c>
+      <c r="I20" t="s">
+        <v>302</v>
+      </c>
+      <c r="J20" t="s">
+        <v>303</v>
+      </c>
+      <c r="K20" t="s">
+        <v>304</v>
+      </c>
+      <c r="M20" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B21" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F21" t="s">
+        <v>306</v>
+      </c>
+      <c r="I21" t="s">
+        <v>307</v>
+      </c>
+      <c r="J21" t="s">
+        <v>308</v>
+      </c>
+      <c r="K21" t="s">
+        <v>309</v>
+      </c>
+      <c r="M21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="F22" t="s">
+        <v>312</v>
+      </c>
+      <c r="I22" t="s">
+        <v>313</v>
+      </c>
+      <c r="K22" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F23" t="s">
+        <v>317</v>
+      </c>
+      <c r="I23" t="s">
+        <v>318</v>
+      </c>
+      <c r="K23" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" t="s">
+        <v>321</v>
+      </c>
+      <c r="I24" t="s">
+        <v>322</v>
+      </c>
+      <c r="K24" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" t="s">
+        <v>325</v>
+      </c>
+      <c r="I25" t="s">
+        <v>326</v>
+      </c>
+      <c r="K25" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I26" t="s">
+        <v>329</v>
+      </c>
+      <c r="K26" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="I27" t="s">
+        <v>332</v>
+      </c>
+      <c r="K27" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="I28" t="s">
+        <v>334</v>
+      </c>
+      <c r="K28" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="I29" t="s">
+        <v>337</v>
+      </c>
+      <c r="K29" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="I30" t="s">
+        <v>340</v>
+      </c>
+      <c r="K30" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="I31" t="s">
+        <v>343</v>
+      </c>
+      <c r="K31" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="I32" t="s">
+        <v>346</v>
+      </c>
+      <c r="K32" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="I33" t="s">
+        <v>348</v>
+      </c>
+      <c r="K33" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="I34" t="s">
+        <v>350</v>
+      </c>
+      <c r="K34" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="I35" t="s">
+        <v>352</v>
+      </c>
+      <c r="K35" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>148</v>
       </c>
+      <c r="B36" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="I36" t="s">
+        <v>354</v>
+      </c>
+      <c r="K36" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I37" t="s">
+        <v>356</v>
+      </c>
+      <c r="K37" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="I38" t="s">
+        <v>359</v>
+      </c>
+      <c r="K38" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I39" t="s">
+        <v>361</v>
+      </c>
+      <c r="K39" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="I40" t="s">
+        <v>363</v>
+      </c>
+      <c r="K40" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I41" t="s">
+        <v>365</v>
+      </c>
+      <c r="K41" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="I42" t="s">
+        <v>367</v>
+      </c>
+      <c r="K42" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="I43" t="s">
+        <v>370</v>
+      </c>
+      <c r="K43" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I44" t="s">
+        <v>373</v>
+      </c>
+      <c r="K44" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I45" t="s">
+        <v>376</v>
+      </c>
+      <c r="K45" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I46" t="s">
+        <v>379</v>
+      </c>
+      <c r="K46" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="I47" t="s">
+        <v>381</v>
+      </c>
+      <c r="K47" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="I48" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="I49" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I50" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="I51" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="I52" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I53" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="I54" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="I55" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="I56" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I57" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I58" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I59" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I60" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I61" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I62" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I63" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I64" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I65" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I66" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="67" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I67" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="68" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I68" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I69" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="70" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I70" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I71" t="s">
+        <v>412</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1564686220" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.787500" right="0.787500" top="0.787500" bottom="0.787500" header="0.393750" footer="0.393750"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1564686220" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1564686220" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.51180599999999998"/>
+  <pageSetup paperSize="9" fitToWidth="0"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:sheetPrefs xmlns:pm="smNativeData" day="1564686220" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">

</xml_diff>

<commit_message>
adding functionality to san_chassis_params.py
</commit_message>
<xml_diff>
--- a/san_automation_info.xlsx
+++ b/san_automation_info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="switch_info" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="460">
   <si>
     <t>switchType</t>
   </si>
@@ -1302,13 +1302,121 @@
   </si>
   <si>
     <t>timezone</t>
+  </si>
+  <si>
+    <t>switch_params_configshow</t>
+  </si>
+  <si>
+    <t>boot.mac</t>
+  </si>
+  <si>
+    <t>boot.gateway.ipa</t>
+  </si>
+  <si>
+    <t>fabric.domain</t>
+  </si>
+  <si>
+    <t>fabric.ops.BBCredit</t>
+  </si>
+  <si>
+    <t>fabric.ops.E_D_TOV</t>
+  </si>
+  <si>
+    <t>fabric.ops.R_A_TOV</t>
+  </si>
+  <si>
+    <t>fabric.ops.bladeFault_on_hwErrlevel</t>
+  </si>
+  <si>
+    <t>fabric.ops.dataFieldSize</t>
+  </si>
+  <si>
+    <t>fabric.ops.max_hops</t>
+  </si>
+  <si>
+    <t>fabric.ops.mode.fcpProbeDisable</t>
+  </si>
+  <si>
+    <t>fabric.ops.mode.isolate</t>
+  </si>
+  <si>
+    <t>fabric.ops.mode.noClassF</t>
+  </si>
+  <si>
+    <t>fabric.ops.mode.tachyonCompat</t>
+  </si>
+  <si>
+    <t>fabric.ops.mode.unicastOnly</t>
+  </si>
+  <si>
+    <t>fabric.ops.mode.useCsCtl</t>
+  </si>
+  <si>
+    <t>fabric.ops.vc.class.2</t>
+  </si>
+  <si>
+    <t>fabric.ops.vc.class.3</t>
+  </si>
+  <si>
+    <t>fabric.ops.vc.config</t>
+  </si>
+  <si>
+    <t>fabric.ops.vc.linkCtrl</t>
+  </si>
+  <si>
+    <t>fabric.ops.vc.multicast</t>
+  </si>
+  <si>
+    <t>fabric.ops.wan_tov</t>
+  </si>
+  <si>
+    <t>rte.external_policy</t>
+  </si>
+  <si>
+    <t>zoning.targetPeerZoning</t>
+  </si>
+  <si>
+    <t>defzone</t>
+  </si>
+  <si>
+    <t>maps.activePolicy</t>
+  </si>
+  <si>
+    <t>ams_maps_log</t>
+  </si>
+  <si>
+    <t>maps.actions</t>
+  </si>
+  <si>
+    <t>switch_index</t>
+  </si>
+  <si>
+    <t>switch_columns_configshow</t>
+  </si>
+  <si>
+    <t>enabled_zoning_config</t>
+  </si>
+  <si>
+    <t>enable</t>
+  </si>
+  <si>
+    <t>cpu_average_load</t>
+  </si>
+  <si>
+    <t>uptime_days</t>
+  </si>
+  <si>
+    <t>flash_usage</t>
+  </si>
+  <si>
+    <t>memory_usage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1320,6 +1428,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1349,7 +1464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1367,6 +1482,9 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -2881,7 +2999,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.51180599999999998"/>
-  <pageSetup paperSize="9" fitToWidth="0"/>
+  <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:sheetPrefs xmlns:pm="smNativeData" day="1564686220" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
@@ -2895,156 +3013,739 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.28515625" customWidth="1"/>
     <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>172</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C2" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="C4" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="C5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="C6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="C7" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="C8" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="C10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>417</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B11" s="10" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="C11" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>418</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B12" s="11" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="C12" s="5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="C13" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B14" s="10" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="C14" s="5" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>146</v>
       </c>
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>147</v>
       </c>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C26" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C27" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C28" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C29" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="13"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="13"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C31" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C32" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="13"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C35" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13"/>
+      <c r="S35" s="13"/>
+      <c r="T35" s="13"/>
+      <c r="U35" s="13"/>
+      <c r="V35" s="13"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C36" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C37" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="13"/>
+      <c r="S37" s="13"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
+      <c r="V37" s="13"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C38" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="13"/>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C39" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13"/>
+      <c r="S39" s="13"/>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13"/>
+      <c r="V39" s="13"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C40" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="13"/>
+      <c r="S40" s="13"/>
+      <c r="T40" s="13"/>
+      <c r="U40" s="13"/>
+      <c r="V40" s="13"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C41" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C42" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="13"/>
+      <c r="V42" s="13"/>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="13"/>
+      <c r="P44" s="13"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="13"/>
+      <c r="T44" s="13"/>
+      <c r="U44" s="13"/>
+      <c r="V44" s="13"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13"/>
+      <c r="V45" s="13"/>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
+      <c r="T46" s="13"/>
+      <c r="U46" s="13"/>
+      <c r="V46" s="13"/>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
@@ -3075,202 +3776,326 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.140625" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="C2" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="7" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>421</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="7" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="7" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>415</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>420</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="7" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="7" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>417</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>418</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>148</v>
+      <c r="B21" s="5"/>
+      <c r="C21" s="7" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="5" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="5" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="5" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="5" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="5" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="5" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="5" t="s">
+        <v>445</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.39374999999999999" footer="0.39374999999999999"/>
-  <pageSetup paperSize="9" fitToWidth="0" pageOrder="overThenDown"/>
+  <pageSetup paperSize="9" fitToWidth="0" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:sheetPrefs xmlns:pm="smNativeData" day="1564686220" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
@@ -4554,7 +5379,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.51180599999999998"/>
-  <pageSetup paperSize="9" fitToWidth="0"/>
+  <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:sheetPrefs xmlns:pm="smNativeData" day="1564686220" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">

</xml_diff>

<commit_message>
add functions to automatic re expressions extract
</commit_message>
<xml_diff>
--- a/san_automation_info.xlsx
+++ b/san_automation_info.xlsx
@@ -9,15 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="switch_info" sheetId="1" r:id="rId1"/>
     <sheet name="parameters" sheetId="2" r:id="rId2"/>
-    <sheet name="columns" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
+    <sheet name="chassis" sheetId="5" r:id="rId3"/>
+    <sheet name="switch" sheetId="7" r:id="rId4"/>
+    <sheet name="columns" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
+    <sheet name="notes" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="4283453520" iterateDelta="1E-4"/>
+  <calcPr calcId="4283453520"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:revision xmlns:pm="smNativeData" day="1564686220" val="966" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="521">
   <si>
     <t>switchType</t>
   </si>
@@ -1410,6 +1413,189 @@
   </si>
   <si>
     <t>memory_usage</t>
+  </si>
+  <si>
+    <t>chassis_param_comp</t>
+  </si>
+  <si>
+    <t>snmp_target_comp</t>
+  </si>
+  <si>
+    <t>syslog_comp</t>
+  </si>
+  <si>
+    <t>memory_comp</t>
+  </si>
+  <si>
+    <t>flash_comp</t>
+  </si>
+  <si>
+    <t>tz_comp</t>
+  </si>
+  <si>
+    <t>uptime_cpu_comp</t>
+  </si>
+  <si>
+    <t>comp_names</t>
+  </si>
+  <si>
+    <t>comp_values</t>
+  </si>
+  <si>
+    <t>lines example</t>
+  </si>
+  <si>
+    <t>Number of LS = 4, system.i2cTurboCnfg:1</t>
+  </si>
+  <si>
+    <t>snmp.snmpv3TrapTarget.0.trapTargetAddr:10.99.245.222</t>
+  </si>
+  <si>
+    <t>syslog.address.1:10.99.116.66</t>
+  </si>
+  <si>
+    <t>ts.tzh:3</t>
+  </si>
+  <si>
+    <t>09:46:50 up 75 days, 22:29, 1 user, load average: 7.38, 3.83, 2.00</t>
+  </si>
+  <si>
+    <t>/dev/root  394440    207140    166940  55% /</t>
+  </si>
+  <si>
+    <t>MemTotal: 504348 kB</t>
+  </si>
+  <si>
+    <t>params_add</t>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>re_names</t>
+  </si>
+  <si>
+    <t>chassis_param</t>
+  </si>
+  <si>
+    <t>snmp_target</t>
+  </si>
+  <si>
+    <t>syslog</t>
+  </si>
+  <si>
+    <t>tz</t>
+  </si>
+  <si>
+    <t>uptime_cpu</t>
+  </si>
+  <si>
+    <t>memory</t>
+  </si>
+  <si>
+    <t>flash</t>
+  </si>
+  <si>
+    <t>^([\w .-]+) ?(=|:) ?([\w. :/]+)$</t>
+  </si>
+  <si>
+    <t>^(snmp.snmpv3TrapTarget.\d.trapTargetAddr):([\d.]+)$</t>
+  </si>
+  <si>
+    <t>^(syslog.address.\d):([\d.]+)$</t>
+  </si>
+  <si>
+    <t>^(ts.tz[hm]):(\d+)$</t>
+  </si>
+  <si>
+    <t>^ [\d: ]+up\s+([\d]+)\s+days,?\s+[\d:]+,\s+[\w ]+,\s+[a-z ]+:\s+[\d.,]+\s+[\d.,]+\s+([\d.]+)$</t>
+  </si>
+  <si>
+    <t>^(\w+):\s+(\d+)\s+kB$</t>
+  </si>
+  <si>
+    <t>^/dev/root\s+\d+\s+\d+\s+\d+\s+(\d+)%\s+/$</t>
+  </si>
+  <si>
+    <t>params_required_to_extract</t>
+  </si>
+  <si>
+    <t>just for informarion</t>
+  </si>
+  <si>
+    <t>parameters list checked with re</t>
+  </si>
+  <si>
+    <t>not imported</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>names for compile and match vars</t>
+  </si>
+  <si>
+    <t>name can be changed but not order</t>
+  </si>
+  <si>
+    <t>but not order</t>
+  </si>
+  <si>
+    <t>from dictionary with all values</t>
+  </si>
+  <si>
+    <t>params names used to form list with req values</t>
+  </si>
+  <si>
+    <t>blue params name can't be chaged</t>
+  </si>
+  <si>
+    <t>new params names could be added</t>
+  </si>
+  <si>
+    <t>additional params to add in dictionary</t>
+  </si>
+  <si>
+    <t>with all values. Added manualy (like configname)</t>
+  </si>
+  <si>
+    <t>or added as combination of ble params like syslog</t>
+  </si>
+  <si>
+    <t>param column</t>
+  </si>
+  <si>
+    <t>to save in excel file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red params names can be changed but only with </t>
+  </si>
+  <si>
+    <t>with param add column</t>
+  </si>
+  <si>
+    <t>column names for dataframe</t>
+  </si>
+  <si>
+    <t>column names can be changed</t>
+  </si>
+  <si>
+    <t>but order has to be same as in param</t>
+  </si>
+  <si>
+    <t>regular expression can be changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red params names can be changed but only </t>
+  </si>
+  <si>
+    <t>^([\w .-]+) ?(=|:) ?([-\w. :/]+)$</t>
+  </si>
+  <si>
+    <t>SwitchName = swDC_62r</t>
+  </si>
+  <si>
+    <t>switch_param</t>
   </si>
 </sst>
 </file>
@@ -1438,7 +1624,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1448,6 +1634,60 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1464,7 +1704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1485,6 +1725,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -3016,7 +3271,7 @@
   <dimension ref="A1:V52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C2" sqref="C2:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3776,10 +4031,998 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="37" style="7" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>487</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>461</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>488</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>471</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>489</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>472</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>465</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>473</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>416</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>466</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>491</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>474</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>463</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>492</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>476</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>464</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>493</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>475</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
+        <v>458</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="36.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>520</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>518</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>426</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>426</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>447</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>448</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>447</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>451</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>448</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>451</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>429</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>431</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>429</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>433</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>431</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>434</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>435</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>433</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>434</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>436</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>435</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>437</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>436</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>438</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>439</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>437</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>440</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>438</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>439</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>440</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>443</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>444</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>445</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>443</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="15" t="s">
+        <v>444</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E42" s="15" t="s">
+        <v>445</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4107,7 +5350,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M71"/>
   <sheetViews>
@@ -5389,4 +6632,153 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" customWidth="1"/>
+    <col min="6" max="6" width="47.28515625" customWidth="1"/>
+    <col min="7" max="7" width="36.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>497</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>498</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>498</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>497</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>498</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>498</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B3" t="s">
+        <v>499</v>
+      </c>
+      <c r="C3" t="s">
+        <v>516</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="E3" t="s">
+        <v>503</v>
+      </c>
+      <c r="F3" t="s">
+        <v>506</v>
+      </c>
+      <c r="G3" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>496</v>
+      </c>
+      <c r="B4" t="s">
+        <v>500</v>
+      </c>
+      <c r="C4" t="s">
+        <v>501</v>
+      </c>
+      <c r="E4" t="s">
+        <v>502</v>
+      </c>
+      <c r="F4" t="s">
+        <v>507</v>
+      </c>
+      <c r="G4" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="F5" t="s">
+        <v>508</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="28" t="s">
+        <v>517</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>511</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="28" t="s">
+        <v>512</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>505</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
portcmd info extract module added
</commit_message>
<xml_diff>
--- a/san_automation_info.xlsx
+++ b/san_automation_info.xlsx
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="switch_info" sheetId="1" r:id="rId1"/>
     <sheet name="chassis" sheetId="5" r:id="rId2"/>
     <sheet name="switch" sheetId="7" r:id="rId3"/>
-    <sheet name="maps" sheetId="8" r:id="rId4"/>
-    <sheet name="fabricshow" sheetId="10" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
-    <sheet name="notes" sheetId="6" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
+    <sheet name="portcmd" sheetId="11" r:id="rId4"/>
+    <sheet name="maps" sheetId="8" r:id="rId5"/>
+    <sheet name="fabricshow" sheetId="10" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId7"/>
+    <sheet name="notes" sheetId="6" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Sheet1!$C$34:$C$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Sheet1!$C$34:$C$66</definedName>
   </definedNames>
-  <calcPr calcId="4283453520"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:revision xmlns:pm="smNativeData" day="1564686220" val="966" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="753">
   <si>
     <t>switchType</t>
   </si>
@@ -2101,6 +2102,201 @@
   </si>
   <si>
     <t>FCRouter_EX_port</t>
+  </si>
+  <si>
+    <t>FC Router DID</t>
+  </si>
+  <si>
+    <t>portState</t>
+  </si>
+  <si>
+    <t>portId</t>
+  </si>
+  <si>
+    <t>portWwn</t>
+  </si>
+  <si>
+    <t>^portFcPortCmdShow --slot (\d{1,2}) (\d{1,2}) \d+$</t>
+  </si>
+  <si>
+    <t>portFcPortCmdShow --slot 10 37 3</t>
+  </si>
+  <si>
+    <t>Credit_Recovery</t>
+  </si>
+  <si>
+    <t>FC_Fastwrite</t>
+  </si>
+  <si>
+    <t>slot_port_number</t>
+  </si>
+  <si>
+    <t>^portshow +(\d{1,4})$</t>
+  </si>
+  <si>
+    <t>portshow 2</t>
+  </si>
+  <si>
+    <t>^([\w ]+): +([\w:.]+) *([\w]+)?:? *(\d+)? *([\w]+)?:? *(\d+)? *$</t>
+  </si>
+  <si>
+    <t>portshow_params</t>
+  </si>
+  <si>
+    <t>^ +[fed]{2} +([\da-f]{6}) +([a-f\d:]+) +[\w= ]+$</t>
+  </si>
+  <si>
+    <t>connected_wwn</t>
+  </si>
+  <si>
+    <t>connected_wwns</t>
+  </si>
+  <si>
+    <t>port_ids</t>
+  </si>
+  <si>
+    <t>^\b(\w+(?&lt;!vc)\b) +([\d-]+)</t>
+  </si>
+  <si>
+    <t>portstats</t>
+  </si>
+  <si>
+    <t>portstats_vc</t>
+  </si>
+  <si>
+    <t>^(\w+)\s{1,2}(\d{1,2})-\s?(\d{1,2}):\s+(\d+)\s+(\d+)\s+(\d+)\s+(\d+)</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_0</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_1</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_2</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_3</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_4</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_5</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_6</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_7</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_8</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_9</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_10</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_11</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_12</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_13</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_14</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc_15</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_0</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_1</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_2</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_3</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_4</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_5</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_6</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_7</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_8</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_9</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_10</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_11</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_12</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_13</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_14</t>
+  </si>
+  <si>
+    <t>tim_latency_vc_15</t>
+  </si>
+  <si>
+    <t>Section: SSHOW_PORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ... rebuilt finished </t>
+  </si>
+  <si>
+    <t>portshow 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ff  131500  50:01:43:80:23:1c:99:34     0     0   8  d_id=FFFFFA</t>
+  </si>
+  <si>
+    <t>F_Trunk: Inactive</t>
+  </si>
+  <si>
+    <t>portloginshow 21</t>
+  </si>
+  <si>
+    <t>stat_wtx 14375003157</t>
+  </si>
+  <si>
+    <t>tim_txcrd_z_vc  0- 3:  0 0  0 0</t>
+  </si>
+  <si>
+    <t>portregshow 21</t>
+  </si>
+  <si>
+    <t>portstatsshow 21</t>
+  </si>
+  <si>
+    <t>portstats64show 21</t>
+  </si>
+  <si>
+    <t>portshow 21</t>
   </si>
 </sst>
 </file>
@@ -2122,7 +2318,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2231,6 +2427,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2244,7 +2458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2288,6 +2502,9 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -3819,7 +4036,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4412,8 +4629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5555,10 +5772,1333 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K106"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="30.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="49" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G2" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>741</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>628</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>628</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>560</v>
+      </c>
+      <c r="B4" s="26">
+        <v>0</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>696</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>693</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>692</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>693</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" s="37">
+        <v>1</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>560</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>698</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>697</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>743</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>704</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>704</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>704</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>703</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>703</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>703</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="B9" s="24">
+        <v>2</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>700</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>699</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>745</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>689</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>690</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>746</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>690</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>691</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>691</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" s="15">
+        <v>3</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>702</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>746</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>701</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>749</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="38">
+        <v>4</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>706</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>750</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>705</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>747</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="39">
+        <v>5</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>707</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>751</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>708</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>748</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="G25" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="G26" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="G27" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="G28" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="G29" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="G30" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="G31" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="G32" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
+        <v>324</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>324</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="G36" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="G37" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="G38" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="G39" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="38" t="s">
+        <v>204</v>
+      </c>
+      <c r="G40" s="38" t="s">
+        <v>204</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="G41" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="38" t="s">
+        <v>222</v>
+      </c>
+      <c r="G42" s="38" t="s">
+        <v>222</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="G43" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="G44" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="G45" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="G46" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="G47" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="39" t="s">
+        <v>709</v>
+      </c>
+      <c r="G48" s="39" t="s">
+        <v>709</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="39" t="s">
+        <v>710</v>
+      </c>
+      <c r="G49" s="39" t="s">
+        <v>710</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="39" t="s">
+        <v>711</v>
+      </c>
+      <c r="G50" s="39" t="s">
+        <v>711</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="39" t="s">
+        <v>712</v>
+      </c>
+      <c r="G51" s="39" t="s">
+        <v>712</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="39" t="s">
+        <v>713</v>
+      </c>
+      <c r="G52" s="39" t="s">
+        <v>713</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="39" t="s">
+        <v>714</v>
+      </c>
+      <c r="G53" s="39" t="s">
+        <v>714</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="39" t="s">
+        <v>715</v>
+      </c>
+      <c r="G54" s="39" t="s">
+        <v>715</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="39" t="s">
+        <v>716</v>
+      </c>
+      <c r="G55" s="39" t="s">
+        <v>716</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="39" t="s">
+        <v>717</v>
+      </c>
+      <c r="G56" s="39" t="s">
+        <v>717</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="39" t="s">
+        <v>718</v>
+      </c>
+      <c r="G57" s="39" t="s">
+        <v>718</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="39" t="s">
+        <v>719</v>
+      </c>
+      <c r="G58" s="39" t="s">
+        <v>719</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="39" t="s">
+        <v>720</v>
+      </c>
+      <c r="G59" s="39" t="s">
+        <v>720</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="39" t="s">
+        <v>721</v>
+      </c>
+      <c r="G60" s="39" t="s">
+        <v>721</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="39" t="s">
+        <v>722</v>
+      </c>
+      <c r="G61" s="39" t="s">
+        <v>722</v>
+      </c>
+      <c r="I61" s="7" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="39" t="s">
+        <v>723</v>
+      </c>
+      <c r="G62" s="39" t="s">
+        <v>723</v>
+      </c>
+      <c r="I62" s="7" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="39" t="s">
+        <v>724</v>
+      </c>
+      <c r="G63" s="39" t="s">
+        <v>724</v>
+      </c>
+      <c r="I63" s="7" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="39" t="s">
+        <v>725</v>
+      </c>
+      <c r="G64" s="39" t="s">
+        <v>725</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="39" t="s">
+        <v>726</v>
+      </c>
+      <c r="G65" s="39" t="s">
+        <v>726</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="39" t="s">
+        <v>727</v>
+      </c>
+      <c r="G66" s="39" t="s">
+        <v>727</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="39" t="s">
+        <v>728</v>
+      </c>
+      <c r="G67" s="39" t="s">
+        <v>728</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="39" t="s">
+        <v>729</v>
+      </c>
+      <c r="G68" s="39" t="s">
+        <v>729</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="39" t="s">
+        <v>730</v>
+      </c>
+      <c r="G69" s="39" t="s">
+        <v>730</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="39" t="s">
+        <v>731</v>
+      </c>
+      <c r="G70" s="39" t="s">
+        <v>731</v>
+      </c>
+      <c r="I70" s="7" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="39" t="s">
+        <v>732</v>
+      </c>
+      <c r="G71" s="39" t="s">
+        <v>732</v>
+      </c>
+      <c r="I71" s="7" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="39" t="s">
+        <v>733</v>
+      </c>
+      <c r="G72" s="39" t="s">
+        <v>733</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="39" t="s">
+        <v>734</v>
+      </c>
+      <c r="G73" s="39" t="s">
+        <v>734</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="39" t="s">
+        <v>735</v>
+      </c>
+      <c r="G74" s="39" t="s">
+        <v>735</v>
+      </c>
+      <c r="I74" s="7" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="39" t="s">
+        <v>736</v>
+      </c>
+      <c r="G75" s="39" t="s">
+        <v>736</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="39" t="s">
+        <v>737</v>
+      </c>
+      <c r="G76" s="39" t="s">
+        <v>737</v>
+      </c>
+      <c r="I76" s="7" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="39" t="s">
+        <v>738</v>
+      </c>
+      <c r="G77" s="39" t="s">
+        <v>738</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="39" t="s">
+        <v>739</v>
+      </c>
+      <c r="G78" s="39" t="s">
+        <v>739</v>
+      </c>
+      <c r="I78" s="7" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="39" t="s">
+        <v>740</v>
+      </c>
+      <c r="G79" s="39" t="s">
+        <v>740</v>
+      </c>
+      <c r="I79" s="7" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="38" t="s">
+        <v>378</v>
+      </c>
+      <c r="G80" s="38" t="s">
+        <v>378</v>
+      </c>
+      <c r="I80" s="7" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="38" t="s">
+        <v>380</v>
+      </c>
+      <c r="G81" s="38" t="s">
+        <v>380</v>
+      </c>
+      <c r="I81" s="7" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="38" t="s">
+        <v>383</v>
+      </c>
+      <c r="G82" s="38" t="s">
+        <v>383</v>
+      </c>
+      <c r="I82" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="38" t="s">
+        <v>386</v>
+      </c>
+      <c r="G83" s="38" t="s">
+        <v>386</v>
+      </c>
+      <c r="I83" s="7" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="38" t="s">
+        <v>388</v>
+      </c>
+      <c r="G84" s="38" t="s">
+        <v>388</v>
+      </c>
+      <c r="I84" s="7" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="38" t="s">
+        <v>390</v>
+      </c>
+      <c r="G85" s="38" t="s">
+        <v>390</v>
+      </c>
+      <c r="I85" s="7" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="38" t="s">
+        <v>392</v>
+      </c>
+      <c r="G86" s="38" t="s">
+        <v>392</v>
+      </c>
+      <c r="I86" s="7" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="38" t="s">
+        <v>393</v>
+      </c>
+      <c r="G87" s="38" t="s">
+        <v>393</v>
+      </c>
+      <c r="I87" s="7" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="38" t="s">
+        <v>394</v>
+      </c>
+      <c r="G88" s="38" t="s">
+        <v>394</v>
+      </c>
+      <c r="I88" s="7" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="38" t="s">
+        <v>395</v>
+      </c>
+      <c r="G89" s="38" t="s">
+        <v>395</v>
+      </c>
+      <c r="I89" s="7" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="38" t="s">
+        <v>396</v>
+      </c>
+      <c r="G90" s="38" t="s">
+        <v>396</v>
+      </c>
+      <c r="I90" s="7" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="38" t="s">
+        <v>397</v>
+      </c>
+      <c r="G91" s="38" t="s">
+        <v>397</v>
+      </c>
+      <c r="I91" s="7" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="38" t="s">
+        <v>398</v>
+      </c>
+      <c r="G92" s="38" t="s">
+        <v>398</v>
+      </c>
+      <c r="I92" s="7" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="38" t="s">
+        <v>399</v>
+      </c>
+      <c r="G93" s="38" t="s">
+        <v>399</v>
+      </c>
+      <c r="I93" s="7" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="38" t="s">
+        <v>400</v>
+      </c>
+      <c r="G94" s="38" t="s">
+        <v>400</v>
+      </c>
+      <c r="I94" s="7" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="38" t="s">
+        <v>401</v>
+      </c>
+      <c r="G95" s="38" t="s">
+        <v>401</v>
+      </c>
+      <c r="I95" s="7" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="38" t="s">
+        <v>402</v>
+      </c>
+      <c r="G96" s="38" t="s">
+        <v>402</v>
+      </c>
+      <c r="I96" s="7" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="38" t="s">
+        <v>403</v>
+      </c>
+      <c r="G97" s="38" t="s">
+        <v>403</v>
+      </c>
+      <c r="I97" s="7" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="G98" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="I98" s="7" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="38" t="s">
+        <v>405</v>
+      </c>
+      <c r="G99" s="38" t="s">
+        <v>405</v>
+      </c>
+      <c r="I99" s="7" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="G100" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="I100" s="7" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="G101" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="I101" s="7" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="38" t="s">
+        <v>408</v>
+      </c>
+      <c r="G102" s="38" t="s">
+        <v>408</v>
+      </c>
+      <c r="I102" s="7" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="38" t="s">
+        <v>409</v>
+      </c>
+      <c r="G103" s="38" t="s">
+        <v>409</v>
+      </c>
+      <c r="I103" s="7" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="38" t="s">
+        <v>410</v>
+      </c>
+      <c r="G104" s="38" t="s">
+        <v>410</v>
+      </c>
+      <c r="I104" s="7" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="38" t="s">
+        <v>411</v>
+      </c>
+      <c r="G105" s="38" t="s">
+        <v>411</v>
+      </c>
+      <c r="I105" s="7" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>742</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5967,12 +7507,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24:K28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6026,10 +7566,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="18" t="s">
         <v>171</v>
       </c>
       <c r="I2" s="12" t="s">
@@ -6037,10 +7577,10 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="18" t="s">
         <v>653</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="18" t="s">
         <v>653</v>
       </c>
       <c r="I3" s="12" t="s">
@@ -6048,10 +7588,10 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="18" t="s">
         <v>448</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="18" t="s">
         <v>448</v>
       </c>
       <c r="I4" s="12" t="s">
@@ -6059,68 +7599,74 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="31" t="s">
         <v>644</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="31">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="31" t="s">
         <v>649</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="31" t="s">
         <v>652</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="31" t="s">
         <v>651</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="18" t="s">
         <v>644</v>
       </c>
+      <c r="H5" s="18"/>
       <c r="I5" s="12" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="31" t="s">
         <v>645</v>
       </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
       <c r="I6" s="7" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="31" t="s">
         <v>646</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="18" t="s">
         <v>645</v>
       </c>
+      <c r="H7" s="18"/>
       <c r="I7" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="31" t="s">
         <v>647</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="18" t="s">
         <v>646</v>
       </c>
+      <c r="H8" s="18"/>
       <c r="I8" s="7" t="s">
         <v>655</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="31" t="s">
         <v>648</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="18" t="s">
         <v>647</v>
       </c>
+      <c r="H9" s="18"/>
       <c r="I9" s="7" t="s">
         <v>656</v>
       </c>
@@ -6136,124 +7682,175 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>674</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>666</v>
-      </c>
-      <c r="E12" t="s">
-        <v>662</v>
-      </c>
-      <c r="F12" t="s">
-        <v>663</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>648</v>
-      </c>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
       <c r="K12" s="12" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>675</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>667</v>
-      </c>
-      <c r="E13" t="s">
-        <v>661</v>
-      </c>
-      <c r="F13" t="s">
-        <v>664</v>
-      </c>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
       <c r="K13" s="12" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>669</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>668</v>
-      </c>
-      <c r="E14" t="s">
-        <v>677</v>
-      </c>
-      <c r="F14" t="s">
-        <v>665</v>
-      </c>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
       <c r="K14" s="12" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>670</v>
-      </c>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
       <c r="K15" s="12" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>671</v>
+      <c r="A16" s="36" t="s">
+        <v>674</v>
+      </c>
+      <c r="B16" s="36">
+        <v>1</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>666</v>
+      </c>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36" t="s">
+        <v>662</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>663</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>648</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>672</v>
-      </c>
+      <c r="A17" s="36" t="s">
+        <v>688</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
       <c r="K17" s="12" t="s">
         <v>685</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>673</v>
-      </c>
-      <c r="D18" t="s">
-        <v>650</v>
+      <c r="A18" s="15" t="s">
+        <v>675</v>
+      </c>
+      <c r="B18" s="15">
+        <v>2</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>667</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15" t="s">
+        <v>661</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>664</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>686</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>669</v>
+      </c>
+      <c r="B19" s="28">
+        <v>3</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>668</v>
+      </c>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28" t="s">
+        <v>677</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>665</v>
+      </c>
       <c r="K19" s="12" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>670</v>
+      </c>
       <c r="K20" s="12" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>671</v>
+      </c>
       <c r="K21" s="12" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>672</v>
+      </c>
       <c r="K22" s="12" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>673</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>650</v>
+      </c>
       <c r="K23" s="12" t="s">
         <v>684</v>
       </c>
@@ -6275,12 +7872,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="I2" sqref="I2:I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7559,7 +9156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -7708,7 +9305,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C25:W83"/>
   <sheetViews>

</xml_diff>

<commit_message>
huawei oceanstore config files parsing
</commit_message>
<xml_diff>
--- a/san_automation_info.xlsx
+++ b/san_automation_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kavlasenko\Documents\05.PYTHON\Projects\san_report_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8529DABB-5C2E-43F9-AA29-25F5757E092B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFC76A5-7899-404F-8F24-C3E625ED0473}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="14" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="1" r:id="rId1"/>
@@ -37,14 +37,15 @@
     <sheet name="blades" sheetId="21" r:id="rId22"/>
     <sheet name="synergy" sheetId="22" r:id="rId23"/>
     <sheet name="3par" sheetId="23" r:id="rId24"/>
-    <sheet name="raslog_details" sheetId="24" r:id="rId25"/>
-    <sheet name="raslog_id_details" sheetId="25" r:id="rId26"/>
-    <sheet name="topology_regex" sheetId="31" r:id="rId27"/>
-    <sheet name="report_columns_links" sheetId="26" r:id="rId28"/>
-    <sheet name="customer_report" sheetId="27" r:id="rId29"/>
-    <sheet name="Sheet1" sheetId="28" r:id="rId30"/>
-    <sheet name="notes" sheetId="29" r:id="rId31"/>
-    <sheet name="Sheet2" sheetId="30" r:id="rId32"/>
+    <sheet name="oceanstor" sheetId="33" r:id="rId25"/>
+    <sheet name="raslog_details" sheetId="24" r:id="rId26"/>
+    <sheet name="raslog_id_details" sheetId="25" r:id="rId27"/>
+    <sheet name="topology_regex" sheetId="31" r:id="rId28"/>
+    <sheet name="report_columns_links" sheetId="26" r:id="rId29"/>
+    <sheet name="customer_report" sheetId="27" r:id="rId30"/>
+    <sheet name="Sheet1" sheetId="28" r:id="rId31"/>
+    <sheet name="notes" sheetId="29" r:id="rId32"/>
+    <sheet name="Sheet2" sheetId="30" r:id="rId33"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">switch_models!$A$3:$L$93</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10968" uniqueCount="4613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11247" uniqueCount="4797">
   <si>
     <t>Contents</t>
   </si>
@@ -14655,6 +14656,578 @@
   </si>
   <si>
     <t>0, 2</t>
+  </si>
+  <si>
+    <t>N(\d+)FC(\d+)</t>
+  </si>
+  <si>
+    <t>N1FC5</t>
+  </si>
+  <si>
+    <t>1, 5</t>
+  </si>
+  <si>
+    <t>infinidat_ctrl_port</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>PROFILE FOR STORAGE ARRAY: +(.+?) +\((.+?)\)</t>
+  </si>
+  <si>
+    <t>storage_profile</t>
+  </si>
+  <si>
+    <t>PROFILE FOR STORAGE ARRAY:  hw01-ost (2023-2-13 16:23:39)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> *(.+?) *: *(.+)</t>
+  </si>
+  <si>
+    <t>Product Model: Dorado6000 V3</t>
+  </si>
+  <si>
+    <t>Os Type:Vmware ESX</t>
+  </si>
+  <si>
+    <t>^ +License-+</t>
+  </si>
+  <si>
+    <t>license_header</t>
+  </si>
+  <si>
+    <t>License------------------------------</t>
+  </si>
+  <si>
+    <t>^ +ID: +CTE.+?MGMT</t>
+  </si>
+  <si>
+    <t>mgmt_eth_id</t>
+  </si>
+  <si>
+    <t>ID: CTE0.SMM0.MGMT</t>
+  </si>
+  <si>
+    <t>ID: CTE0.A.MGMT</t>
+  </si>
+  <si>
+    <t>ID: CTE0.B.MGMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +IPv4 +Address\: +(.+)</t>
+  </si>
+  <si>
+    <t>ip_addr</t>
+  </si>
+  <si>
+    <t>IPv4 Address: 10.221.5.155</t>
+  </si>
+  <si>
+    <t>IPv4 Gateway: 10.221.5.1</t>
+  </si>
+  <si>
+    <t>MAC: 80:e1:bf:08:04:69</t>
+  </si>
+  <si>
+    <t>gateway_mac</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +(IPv4 +Gateway|MAC)\: +.+</t>
+  </si>
+  <si>
+    <t>^FC +Port-+</t>
+  </si>
+  <si>
+    <t>^ +FC +Port-+</t>
+  </si>
+  <si>
+    <t>^ +ID\: +[\w\.]+</t>
+  </si>
+  <si>
+    <t>storage_grouped_fcports_header</t>
+  </si>
+  <si>
+    <t>controller_grouped_fcports_header</t>
+  </si>
+  <si>
+    <t>port_id</t>
+  </si>
+  <si>
+    <t>FC Port--------------------------------</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    FC Port----------------------------------</t>
+  </si>
+  <si>
+    <t>ID: CTE0.IOM.H2.P0</t>
+  </si>
+  <si>
+    <t>^ *(SAS|ETH) +Port-+</t>
+  </si>
+  <si>
+    <t>SAS Port--------------------------------</t>
+  </si>
+  <si>
+    <t>ETH Port--------------------------------</t>
+  </si>
+  <si>
+    <t>^\s*$</t>
+  </si>
+  <si>
+    <t>(^\s*$)|(sfp +info)</t>
+  </si>
+  <si>
+    <t>blank_line</t>
+  </si>
+  <si>
+    <t>blank_or_sfpinfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    sfp info:</t>
+  </si>
+  <si>
+    <t>^Host-+</t>
+  </si>
+  <si>
+    <t>^(Host +Group|Power)-+</t>
+  </si>
+  <si>
+    <t>host_header</t>
+  </si>
+  <si>
+    <t>hostgroup_or_power_header</t>
+  </si>
+  <si>
+    <t>Host--------------------------------</t>
+  </si>
+  <si>
+    <t>Host Group--------------------------------</t>
+  </si>
+  <si>
+    <t>Power--------------------------------</t>
+  </si>
+  <si>
+    <t>sas_eth_port_header</t>
+  </si>
+  <si>
+    <t>^(\d+) +([\w\.-]+) +([\w\.-]+) +([\w\.-]+) +([\w\.-]+) +([\w\.-]+) +([\w\.-]+) +([\w\.-]*) +</t>
+  </si>
+  <si>
+    <t>host_id_name_line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 ESXI02 VMware_ESX  -- -- Balanced  --                                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Host17 VMware_ESX  -- --  Balanced  --  Normal               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">59 n02.s3.dtln.ru  Linux  -- -- Asymmetric No                               </t>
+  </si>
+  <si>
+    <t>^ +Host +\d+-+</t>
+  </si>
+  <si>
+    <t>host_id_header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Host 0--------------------------------</t>
+  </si>
+  <si>
+    <t>^FC +Initiator-+</t>
+  </si>
+  <si>
+    <t>^SFP-+</t>
+  </si>
+  <si>
+    <t>fcinitiator_header</t>
+  </si>
+  <si>
+    <t>sfp_header</t>
+  </si>
+  <si>
+    <t>FC Initiator--------------------------------</t>
+  </si>
+  <si>
+    <t>SFP--------------------------------</t>
+  </si>
+  <si>
+    <t>^(\w+) +([\d-]+) +([\w-]+) +([\w-]+) +([\w-]+) +([\w-]+) +([\w-]+)</t>
+  </si>
+  <si>
+    <t>host_id_fcinitiator_line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100000109b261ebe 0 Offline Default  -- -- --                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">100000109b89e8c0 72 Online Default -- -- --                     </t>
+  </si>
+  <si>
+    <t>^ +Mapping View +INFO</t>
+  </si>
+  <si>
+    <t>host_mapping_header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Mapping View INFO:</t>
+  </si>
+  <si>
+    <t>^ +WWN\: *([\w]+)</t>
+  </si>
+  <si>
+    <t>hostport_wwn</t>
+  </si>
+  <si>
+    <t>WWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     WWN: 0x210034800d6e7f22</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Huawei OceanSto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>r parsing regex patterns</t>
+    </r>
+  </si>
+  <si>
+    <t>config_datetime</t>
+  </si>
+  <si>
+    <t>Product Serial Number</t>
+  </si>
+  <si>
+    <t>Product Model</t>
+  </si>
+  <si>
+    <t>Product Version</t>
+  </si>
+  <si>
+    <t>Patch Version</t>
+  </si>
+  <si>
+    <t>System Location</t>
+  </si>
+  <si>
+    <t>System Description</t>
+  </si>
+  <si>
+    <t>Master CPU Usage</t>
+  </si>
+  <si>
+    <t>Number of total controllers</t>
+  </si>
+  <si>
+    <t>Number of normal controllers</t>
+  </si>
+  <si>
+    <t>Number of disk domains</t>
+  </si>
+  <si>
+    <t>Number of storage pools</t>
+  </si>
+  <si>
+    <t>System max LUN number</t>
+  </si>
+  <si>
+    <t>Total number of LUN</t>
+  </si>
+  <si>
+    <t>Cache low water marker</t>
+  </si>
+  <si>
+    <t>Cache high water marker</t>
+  </si>
+  <si>
+    <t>RUN TIME</t>
+  </si>
+  <si>
+    <t>storage summary section end</t>
+  </si>
+  <si>
+    <t>mgmt interface section start</t>
+  </si>
+  <si>
+    <t>storage profile and summary section start</t>
+  </si>
+  <si>
+    <t>oceanstor details extract</t>
+  </si>
+  <si>
+    <t>IP_Address extract</t>
+  </si>
+  <si>
+    <t>mgmt interface section end</t>
+  </si>
+  <si>
+    <t>Product_Serial_Number</t>
+  </si>
+  <si>
+    <t>Product_Model</t>
+  </si>
+  <si>
+    <t>Product_Version</t>
+  </si>
+  <si>
+    <t>Patch_Version</t>
+  </si>
+  <si>
+    <t>System_Location</t>
+  </si>
+  <si>
+    <t>System_Description</t>
+  </si>
+  <si>
+    <t>Master_CPU_Usage</t>
+  </si>
+  <si>
+    <t>Number_of_total_controllers</t>
+  </si>
+  <si>
+    <t>Number_of_normal_controllers</t>
+  </si>
+  <si>
+    <t>Number_of_disk_domains</t>
+  </si>
+  <si>
+    <t>Number_of_storage_pools</t>
+  </si>
+  <si>
+    <t>System_max_LUN_number</t>
+  </si>
+  <si>
+    <t>Total_number_of_LUN</t>
+  </si>
+  <si>
+    <t>Cache_low_water_marker</t>
+  </si>
+  <si>
+    <t>Cache_high_water_marker</t>
+  </si>
+  <si>
+    <t>Run_time</t>
+  </si>
+  <si>
+    <t>fcport_params</t>
+  </si>
+  <si>
+    <t>fcport_columns</t>
+  </si>
+  <si>
+    <t>controller fcports section start (several in configfile)</t>
+  </si>
+  <si>
+    <t>storage fcports section start (single in configfile)</t>
+  </si>
+  <si>
+    <t>port id (port parameters section start)</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Health Status</t>
+  </si>
+  <si>
+    <t>Running Status</t>
+  </si>
+  <si>
+    <t>SFP Status</t>
+  </si>
+  <si>
+    <t>Working Rate(Mbps)</t>
+  </si>
+  <si>
+    <t>Configured Speed(Mbps)</t>
+  </si>
+  <si>
+    <t>Max Speed(Mbps)</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Health_Status</t>
+  </si>
+  <si>
+    <t>Running_Status</t>
+  </si>
+  <si>
+    <t>SFP_Status</t>
+  </si>
+  <si>
+    <t>Working_Rate(Mbps)</t>
+  </si>
+  <si>
+    <t>Configured_Speed(Mbps)</t>
+  </si>
+  <si>
+    <t>Max_Speed(Mbps)</t>
+  </si>
+  <si>
+    <t>fcports group section end (both for storage and controller type)</t>
+  </si>
+  <si>
+    <t>fcport details section end (sfp details section)</t>
+  </si>
+  <si>
+    <t>controller fcport details extract</t>
+  </si>
+  <si>
+    <t>hostname and hostid extract</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Os Type</t>
+  </si>
+  <si>
+    <t>Ip</t>
+  </si>
+  <si>
+    <t>host_params</t>
+  </si>
+  <si>
+    <t>Operating System</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>ALUA MODE</t>
+  </si>
+  <si>
+    <t>HyperMetro Path Optimized</t>
+  </si>
+  <si>
+    <t>ALUA_MODE</t>
+  </si>
+  <si>
+    <t>HyperMetro_Path_Optimized</t>
+  </si>
+  <si>
+    <t>host and host fcport details extract</t>
+  </si>
+  <si>
+    <t>Name: v4c2h01.dtln.ru</t>
+  </si>
+  <si>
+    <t>Id: 0</t>
+  </si>
+  <si>
+    <t>hosts section start</t>
+  </si>
+  <si>
+    <t>host (single) section start</t>
+  </si>
+  <si>
+    <t>host details (single) section end</t>
+  </si>
+  <si>
+    <t>single host wwn extract</t>
+  </si>
+  <si>
+    <t>Os_Type</t>
+  </si>
+  <si>
+    <t>Host_IP</t>
+  </si>
+  <si>
+    <t>hosts section end</t>
+  </si>
+  <si>
+    <t>Host Id</t>
+  </si>
+  <si>
+    <t>Multipath Type</t>
+  </si>
+  <si>
+    <t>Failover Mode</t>
+  </si>
+  <si>
+    <t>Path Type</t>
+  </si>
+  <si>
+    <t>Special Mode Type</t>
+  </si>
+  <si>
+    <t>host ports section start</t>
+  </si>
+  <si>
+    <t>hostid and host fcport extract</t>
+  </si>
+  <si>
+    <t>Multipath_Type</t>
+  </si>
+  <si>
+    <t>Failover_Mode</t>
+  </si>
+  <si>
+    <t>Path_Type</t>
+  </si>
+  <si>
+    <t>Special_Mode_Type</t>
+  </si>
+  <si>
+    <t>host ports section end</t>
+  </si>
+  <si>
+    <t>hostid_name_columns</t>
+  </si>
+  <si>
+    <t>hostid_fcinitiator_columns</t>
+  </si>
+  <si>
+    <t>ID: CTE0.A.IOM0.P0</t>
+  </si>
+  <si>
+    <t>WWN: 2000048c16ed9856</t>
+  </si>
+  <si>
+    <t>Running Status: Link Up</t>
+  </si>
+  <si>
+    <t>Health Status: Normal</t>
+  </si>
+  <si>
+    <t>Role: INI and TGT</t>
+  </si>
+  <si>
+    <t>Working Rate(Mbps): 16000</t>
+  </si>
+  <si>
+    <t>Max Speed(Mbps): 32000</t>
+  </si>
+  <si>
+    <t>Configured Speed(Mbps): Auto-Adapt</t>
+  </si>
+  <si>
+    <t>SFP Status: Online</t>
+  </si>
+  <si>
+    <t>Type: Host Port</t>
+  </si>
+  <si>
+    <t>Point Release</t>
   </si>
 </sst>
 </file>
@@ -14748,7 +15321,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="50">
+  <fills count="54">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -15043,6 +15616,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -15072,7 +15669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -15202,12 +15799,28 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="49" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="52" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="53" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -15859,7 +16472,7 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17519,8 +18132,8 @@
   <dimension ref="A1:K222"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
+      <pane ySplit="3" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22578,9 +23191,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F152" sqref="F152"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24011,12 +24624,41 @@
         <v>4611</v>
       </c>
     </row>
+    <row r="156" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>2240</v>
+      </c>
+      <c r="C156" t="s">
+        <v>2241</v>
+      </c>
+      <c r="D156">
+        <v>38</v>
+      </c>
+      <c r="E156" t="s">
+        <v>4616</v>
+      </c>
+      <c r="F156" s="24" t="s">
+        <v>2191</v>
+      </c>
+      <c r="G156" t="s">
+        <v>4613</v>
+      </c>
+      <c r="H156" t="s">
+        <v>4614</v>
+      </c>
+      <c r="I156" t="s">
+        <v>4615</v>
+      </c>
+    </row>
     <row r="161" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I161" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E1048576 G154">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+  <conditionalFormatting sqref="E2:E155 G154 E157:E1048576">
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E156 G156:I156">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="contents!A1" display="Contents" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
@@ -25805,7 +26447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26097,7 +26739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -30001,7 +30643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -32201,13 +32843,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:U79"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="53.28515625" customWidth="1"/>
     <col min="2" max="2" width="40.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
@@ -32976,6 +33616,9 @@
       <c r="J43" t="s">
         <v>2926</v>
       </c>
+      <c r="L43" t="s">
+        <v>4617</v>
+      </c>
       <c r="P43" s="64"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
@@ -33289,6 +33932,1258 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2713A8-6D59-46D9-B74D-925022F8954D}">
+  <dimension ref="A1:Q107"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="48.140625" customWidth="1"/>
+    <col min="7" max="7" width="57.85546875" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
+    <col min="10" max="10" width="26" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="24" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" customWidth="1"/>
+    <col min="16" max="17" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="81" t="s">
+        <v>4689</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>2860</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>2861</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>2862</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>4729</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>4730</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>4755</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>2864</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>4784</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>4785</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="95" t="s">
+        <v>4709</v>
+      </c>
+      <c r="B5" s="95" t="s">
+        <v>4690</v>
+      </c>
+      <c r="C5" s="95">
+        <v>0</v>
+      </c>
+      <c r="D5" s="95" t="s">
+        <v>4619</v>
+      </c>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95" t="s">
+        <v>4618</v>
+      </c>
+      <c r="G5" s="96" t="s">
+        <v>4620</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="97" t="s">
+        <v>4710</v>
+      </c>
+      <c r="B7" s="97"/>
+      <c r="C7" s="97">
+        <v>1</v>
+      </c>
+      <c r="D7" s="97" t="s">
+        <v>2885</v>
+      </c>
+      <c r="E7" s="97"/>
+      <c r="F7" s="97" t="s">
+        <v>4621</v>
+      </c>
+      <c r="G7" s="97" t="s">
+        <v>4622</v>
+      </c>
+      <c r="H7" s="100" t="s">
+        <v>901</v>
+      </c>
+      <c r="I7" s="100" t="s">
+        <v>901</v>
+      </c>
+      <c r="J7" s="100" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="97" t="s">
+        <v>2884</v>
+      </c>
+      <c r="G8" s="97" t="s">
+        <v>4623</v>
+      </c>
+      <c r="H8" s="97" t="s">
+        <v>2884</v>
+      </c>
+      <c r="J8" s="97" t="s">
+        <v>2891</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="97" t="s">
+        <v>4691</v>
+      </c>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97" t="s">
+        <v>4691</v>
+      </c>
+      <c r="J9" s="97" t="s">
+        <v>4713</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="97" t="s">
+        <v>4692</v>
+      </c>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97" t="s">
+        <v>4692</v>
+      </c>
+      <c r="J10" s="97" t="s">
+        <v>4714</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="97" t="s">
+        <v>4693</v>
+      </c>
+      <c r="G11" s="97"/>
+      <c r="H11" s="97" t="s">
+        <v>4693</v>
+      </c>
+      <c r="J11" s="97" t="s">
+        <v>4715</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="97" t="s">
+        <v>4796</v>
+      </c>
+      <c r="G12" s="97"/>
+      <c r="H12" s="97" t="s">
+        <v>4796</v>
+      </c>
+      <c r="J12" s="97" t="s">
+        <v>4796</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="97" t="s">
+        <v>4694</v>
+      </c>
+      <c r="G13" s="97"/>
+      <c r="H13" s="97" t="s">
+        <v>4694</v>
+      </c>
+      <c r="J13" s="97" t="s">
+        <v>4716</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="80" t="s">
+        <v>2778</v>
+      </c>
+      <c r="I14" s="80" t="s">
+        <v>2778</v>
+      </c>
+      <c r="J14" s="80" t="s">
+        <v>2778</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="97" t="s">
+        <v>4695</v>
+      </c>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97" t="s">
+        <v>4695</v>
+      </c>
+      <c r="J15" s="97" t="s">
+        <v>4717</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="97" t="s">
+        <v>4696</v>
+      </c>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97" t="s">
+        <v>4696</v>
+      </c>
+      <c r="J16" s="97" t="s">
+        <v>4718</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="97" t="s">
+        <v>4697</v>
+      </c>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97" t="s">
+        <v>4697</v>
+      </c>
+      <c r="J17" s="97" t="s">
+        <v>4719</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="97" t="s">
+        <v>4698</v>
+      </c>
+      <c r="G18" s="97"/>
+      <c r="H18" s="97" t="s">
+        <v>4698</v>
+      </c>
+      <c r="J18" s="97" t="s">
+        <v>4720</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="97" t="s">
+        <v>4699</v>
+      </c>
+      <c r="G19" s="97"/>
+      <c r="H19" s="97" t="s">
+        <v>4699</v>
+      </c>
+      <c r="J19" s="97" t="s">
+        <v>4721</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="97" t="s">
+        <v>4700</v>
+      </c>
+      <c r="G20" s="97"/>
+      <c r="H20" s="97" t="s">
+        <v>4700</v>
+      </c>
+      <c r="J20" s="97" t="s">
+        <v>4722</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="97" t="s">
+        <v>4701</v>
+      </c>
+      <c r="G21" s="97"/>
+      <c r="H21" s="97" t="s">
+        <v>4701</v>
+      </c>
+      <c r="J21" s="97" t="s">
+        <v>4723</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="97" t="s">
+        <v>4702</v>
+      </c>
+      <c r="G22" s="97"/>
+      <c r="H22" s="97" t="s">
+        <v>4702</v>
+      </c>
+      <c r="J22" s="97" t="s">
+        <v>4724</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="97" t="s">
+        <v>4703</v>
+      </c>
+      <c r="G23" s="97"/>
+      <c r="H23" s="97" t="s">
+        <v>4703</v>
+      </c>
+      <c r="J23" s="97" t="s">
+        <v>4725</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="97" t="s">
+        <v>4704</v>
+      </c>
+      <c r="G24" s="97"/>
+      <c r="H24" s="97" t="s">
+        <v>4704</v>
+      </c>
+      <c r="J24" s="97" t="s">
+        <v>4726</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="97" t="s">
+        <v>4705</v>
+      </c>
+      <c r="G25" s="97"/>
+      <c r="H25" s="97" t="s">
+        <v>4705</v>
+      </c>
+      <c r="J25" s="97" t="s">
+        <v>4727</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="97" t="s">
+        <v>4706</v>
+      </c>
+      <c r="G26" s="97"/>
+      <c r="H26" s="97" t="s">
+        <v>4706</v>
+      </c>
+      <c r="J26" s="97" t="s">
+        <v>4728</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G27" s="97"/>
+      <c r="H27" s="80" t="s">
+        <v>4690</v>
+      </c>
+      <c r="I27" s="80" t="s">
+        <v>4690</v>
+      </c>
+      <c r="J27" s="80" t="s">
+        <v>4690</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="98" t="s">
+        <v>4707</v>
+      </c>
+      <c r="B29" s="98"/>
+      <c r="C29" s="98">
+        <v>2</v>
+      </c>
+      <c r="D29" s="98" t="s">
+        <v>4625</v>
+      </c>
+      <c r="E29" s="98"/>
+      <c r="F29" s="98" t="s">
+        <v>4624</v>
+      </c>
+      <c r="G29" s="98" t="s">
+        <v>4626</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="98" t="s">
+        <v>4708</v>
+      </c>
+      <c r="B31" s="98"/>
+      <c r="C31" s="98">
+        <v>3</v>
+      </c>
+      <c r="D31" s="98" t="s">
+        <v>4628</v>
+      </c>
+      <c r="E31" s="98"/>
+      <c r="F31" s="98" t="s">
+        <v>4627</v>
+      </c>
+      <c r="G31" s="98" t="s">
+        <v>4629</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G32" s="98" t="s">
+        <v>4630</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G33" s="98" t="s">
+        <v>4631</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="83" t="s">
+        <v>4711</v>
+      </c>
+      <c r="B35" s="83" t="s">
+        <v>2778</v>
+      </c>
+      <c r="C35" s="83">
+        <v>4</v>
+      </c>
+      <c r="D35" s="83" t="s">
+        <v>4633</v>
+      </c>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83" t="s">
+        <v>4632</v>
+      </c>
+      <c r="G35" s="83" t="s">
+        <v>4634</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="98" t="s">
+        <v>4712</v>
+      </c>
+      <c r="B37" s="98"/>
+      <c r="C37" s="98">
+        <v>5</v>
+      </c>
+      <c r="D37" s="98" t="s">
+        <v>4637</v>
+      </c>
+      <c r="E37" s="98"/>
+      <c r="F37" s="98" t="s">
+        <v>4638</v>
+      </c>
+      <c r="G37" s="98" t="s">
+        <v>4635</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G38" s="98" t="s">
+        <v>4636</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="98" t="s">
+        <v>4732</v>
+      </c>
+      <c r="B40" s="98"/>
+      <c r="C40" s="98">
+        <v>6</v>
+      </c>
+      <c r="D40" s="98" t="s">
+        <v>4642</v>
+      </c>
+      <c r="E40" s="98"/>
+      <c r="F40" s="98" t="s">
+        <v>4639</v>
+      </c>
+      <c r="G40" s="98" t="s">
+        <v>4645</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="98" t="s">
+        <v>4731</v>
+      </c>
+      <c r="B42" s="98"/>
+      <c r="C42" s="98">
+        <v>7</v>
+      </c>
+      <c r="D42" s="98" t="s">
+        <v>4643</v>
+      </c>
+      <c r="E42" s="98"/>
+      <c r="F42" s="98" t="s">
+        <v>4640</v>
+      </c>
+      <c r="G42" s="98" t="s">
+        <v>4646</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="98" t="s">
+        <v>4733</v>
+      </c>
+      <c r="B44" s="98"/>
+      <c r="C44" s="98">
+        <v>8</v>
+      </c>
+      <c r="D44" s="98" t="s">
+        <v>4644</v>
+      </c>
+      <c r="E44" s="98"/>
+      <c r="F44" s="98" t="s">
+        <v>4641</v>
+      </c>
+      <c r="G44" s="98" t="s">
+        <v>4647</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="91"/>
+      <c r="P46"/>
+    </row>
+    <row r="47" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="97" t="s">
+        <v>4750</v>
+      </c>
+      <c r="B47" s="97"/>
+      <c r="C47" s="97"/>
+      <c r="D47" s="97"/>
+      <c r="E47" s="97"/>
+      <c r="F47" s="97"/>
+      <c r="G47" s="97"/>
+      <c r="L47"/>
+      <c r="M47" s="100" t="s">
+        <v>901</v>
+      </c>
+      <c r="P47"/>
+    </row>
+    <row r="48" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="97" t="s">
+        <v>4734</v>
+      </c>
+      <c r="G48" s="97" t="s">
+        <v>4786</v>
+      </c>
+      <c r="L48" s="97" t="s">
+        <v>4734</v>
+      </c>
+      <c r="M48" s="97" t="s">
+        <v>4734</v>
+      </c>
+      <c r="P48"/>
+    </row>
+    <row r="49" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="97" t="s">
+        <v>4687</v>
+      </c>
+      <c r="G49" s="97" t="s">
+        <v>4787</v>
+      </c>
+      <c r="L49" s="97" t="s">
+        <v>4687</v>
+      </c>
+      <c r="M49" s="97" t="s">
+        <v>4687</v>
+      </c>
+      <c r="P49"/>
+    </row>
+    <row r="50" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="97" t="s">
+        <v>4735</v>
+      </c>
+      <c r="G50" s="97" t="s">
+        <v>4789</v>
+      </c>
+      <c r="L50" s="97" t="s">
+        <v>4735</v>
+      </c>
+      <c r="M50" s="97" t="s">
+        <v>4742</v>
+      </c>
+      <c r="P50"/>
+    </row>
+    <row r="51" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="97" t="s">
+        <v>4736</v>
+      </c>
+      <c r="G51" s="97" t="s">
+        <v>4788</v>
+      </c>
+      <c r="L51" s="97" t="s">
+        <v>4736</v>
+      </c>
+      <c r="M51" s="97" t="s">
+        <v>4743</v>
+      </c>
+      <c r="P51"/>
+    </row>
+    <row r="52" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="97" t="s">
+        <v>4737</v>
+      </c>
+      <c r="G52" s="97" t="s">
+        <v>4794</v>
+      </c>
+      <c r="L52" s="97" t="s">
+        <v>4737</v>
+      </c>
+      <c r="M52" s="97" t="s">
+        <v>4744</v>
+      </c>
+      <c r="P52"/>
+    </row>
+    <row r="53" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="97" t="s">
+        <v>2019</v>
+      </c>
+      <c r="G53" s="97" t="s">
+        <v>4795</v>
+      </c>
+      <c r="L53" s="97" t="s">
+        <v>2019</v>
+      </c>
+      <c r="M53" s="97" t="s">
+        <v>2019</v>
+      </c>
+      <c r="P53"/>
+    </row>
+    <row r="54" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="97" t="s">
+        <v>4738</v>
+      </c>
+      <c r="G54" s="97" t="s">
+        <v>4791</v>
+      </c>
+      <c r="L54" s="97" t="s">
+        <v>4738</v>
+      </c>
+      <c r="M54" s="97" t="s">
+        <v>4745</v>
+      </c>
+      <c r="P54"/>
+    </row>
+    <row r="55" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="97" t="s">
+        <v>4739</v>
+      </c>
+      <c r="G55" s="97" t="s">
+        <v>4793</v>
+      </c>
+      <c r="L55" s="97" t="s">
+        <v>4739</v>
+      </c>
+      <c r="M55" s="97" t="s">
+        <v>4746</v>
+      </c>
+      <c r="P55"/>
+    </row>
+    <row r="56" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="97" t="s">
+        <v>4740</v>
+      </c>
+      <c r="G56" s="97" t="s">
+        <v>4792</v>
+      </c>
+      <c r="L56" s="97" t="s">
+        <v>4740</v>
+      </c>
+      <c r="M56" s="97" t="s">
+        <v>4747</v>
+      </c>
+      <c r="P56"/>
+    </row>
+    <row r="57" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="97" t="s">
+        <v>4741</v>
+      </c>
+      <c r="G57" s="97" t="s">
+        <v>4790</v>
+      </c>
+      <c r="L57" s="97" t="s">
+        <v>4741</v>
+      </c>
+      <c r="M57" s="97" t="s">
+        <v>4741</v>
+      </c>
+      <c r="P57"/>
+    </row>
+    <row r="58" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="98" t="s">
+        <v>4748</v>
+      </c>
+      <c r="B59" s="98"/>
+      <c r="C59" s="98">
+        <v>9</v>
+      </c>
+      <c r="D59" s="98" t="s">
+        <v>4663</v>
+      </c>
+      <c r="E59" s="98"/>
+      <c r="F59" s="98" t="s">
+        <v>4648</v>
+      </c>
+      <c r="G59" s="98" t="s">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G60" s="98" t="s">
+        <v>4649</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" s="98"/>
+      <c r="B62" s="98"/>
+      <c r="C62" s="98">
+        <v>10</v>
+      </c>
+      <c r="D62" s="98" t="s">
+        <v>4653</v>
+      </c>
+      <c r="E62" s="98"/>
+      <c r="F62" s="98" t="s">
+        <v>4651</v>
+      </c>
+      <c r="G62" s="98"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="98" t="s">
+        <v>4749</v>
+      </c>
+      <c r="B64" s="98"/>
+      <c r="C64" s="98">
+        <v>11</v>
+      </c>
+      <c r="D64" s="98" t="s">
+        <v>4654</v>
+      </c>
+      <c r="E64" s="98"/>
+      <c r="F64" s="98" t="s">
+        <v>4652</v>
+      </c>
+      <c r="G64" s="98" t="s">
+        <v>4655</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="98" t="s">
+        <v>4765</v>
+      </c>
+      <c r="B66" s="98"/>
+      <c r="C66" s="98">
+        <v>12</v>
+      </c>
+      <c r="D66" s="98" t="s">
+        <v>4658</v>
+      </c>
+      <c r="E66" s="98"/>
+      <c r="F66" s="98" t="s">
+        <v>4656</v>
+      </c>
+      <c r="G66" s="98" t="s">
+        <v>4660</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="98" t="s">
+        <v>4766</v>
+      </c>
+      <c r="B68" s="98"/>
+      <c r="C68" s="98">
+        <v>13</v>
+      </c>
+      <c r="D68" s="98" t="s">
+        <v>4670</v>
+      </c>
+      <c r="E68" s="98"/>
+      <c r="F68" s="98" t="s">
+        <v>4669</v>
+      </c>
+      <c r="G68" s="98" t="s">
+        <v>4671</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="86"/>
+      <c r="B69" s="86"/>
+      <c r="C69" s="86"/>
+      <c r="D69" s="86"/>
+      <c r="E69" s="86"/>
+      <c r="F69" s="86"/>
+      <c r="G69" s="86"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="97" t="s">
+        <v>4762</v>
+      </c>
+      <c r="B70" s="97"/>
+      <c r="C70" s="97"/>
+      <c r="D70" s="97"/>
+      <c r="E70" s="97"/>
+      <c r="F70" s="97"/>
+      <c r="G70" s="97" t="s">
+        <v>4764</v>
+      </c>
+      <c r="N70" s="91"/>
+      <c r="O70" s="100" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="86"/>
+      <c r="B71" s="97" t="s">
+        <v>4752</v>
+      </c>
+      <c r="C71" s="86"/>
+      <c r="D71" s="86"/>
+      <c r="E71" s="86"/>
+      <c r="F71" s="86"/>
+      <c r="G71" s="97" t="s">
+        <v>4763</v>
+      </c>
+      <c r="N71" s="97" t="s">
+        <v>4752</v>
+      </c>
+      <c r="O71" s="97" t="s">
+        <v>2952</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="86"/>
+      <c r="B72" s="97" t="s">
+        <v>2536</v>
+      </c>
+      <c r="C72" s="86"/>
+      <c r="D72" s="86"/>
+      <c r="E72" s="86"/>
+      <c r="F72" s="86"/>
+      <c r="G72" s="97" t="s">
+        <v>4623</v>
+      </c>
+      <c r="N72" s="97" t="s">
+        <v>2536</v>
+      </c>
+      <c r="O72" s="97" t="s">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" s="86"/>
+      <c r="B73" s="97" t="s">
+        <v>4753</v>
+      </c>
+      <c r="C73" s="86"/>
+      <c r="D73" s="86"/>
+      <c r="E73" s="86"/>
+      <c r="F73" s="86"/>
+      <c r="G73" s="86"/>
+      <c r="N73" s="97" t="s">
+        <v>4753</v>
+      </c>
+      <c r="O73" s="97" t="s">
+        <v>4769</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" s="86"/>
+      <c r="B74" s="97" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C74" s="86"/>
+      <c r="D74" s="86"/>
+      <c r="E74" s="86"/>
+      <c r="F74" s="86"/>
+      <c r="G74" s="86"/>
+      <c r="N74" s="97" t="s">
+        <v>4754</v>
+      </c>
+      <c r="O74" s="97" t="s">
+        <v>4770</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="86"/>
+      <c r="B75" s="97" t="s">
+        <v>2921</v>
+      </c>
+      <c r="C75" s="86"/>
+      <c r="D75" s="86"/>
+      <c r="E75" s="86"/>
+      <c r="F75" s="86"/>
+      <c r="G75" s="86"/>
+      <c r="N75" s="97" t="s">
+        <v>2921</v>
+      </c>
+      <c r="O75" s="97" t="s">
+        <v>2921</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="86"/>
+      <c r="B76" s="86"/>
+      <c r="C76" s="86"/>
+      <c r="D76" s="86"/>
+      <c r="E76" s="86"/>
+      <c r="F76" s="86"/>
+      <c r="G76" s="86"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" s="98" t="s">
+        <v>4767</v>
+      </c>
+      <c r="B77" s="98"/>
+      <c r="C77" s="98">
+        <v>14</v>
+      </c>
+      <c r="D77" s="98" t="s">
+        <v>4683</v>
+      </c>
+      <c r="E77" s="98"/>
+      <c r="F77" s="98" t="s">
+        <v>4682</v>
+      </c>
+      <c r="G77" s="98" t="s">
+        <v>4684</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A79" s="97" t="s">
+        <v>4768</v>
+      </c>
+      <c r="B79" s="97" t="s">
+        <v>4687</v>
+      </c>
+      <c r="C79" s="97">
+        <v>15</v>
+      </c>
+      <c r="D79" s="97" t="s">
+        <v>4686</v>
+      </c>
+      <c r="E79" s="97"/>
+      <c r="F79" s="97" t="s">
+        <v>4685</v>
+      </c>
+      <c r="G79" s="97" t="s">
+        <v>4688</v>
+      </c>
+      <c r="O79" s="97" t="s">
+        <v>2961</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" s="86"/>
+      <c r="B80" s="86"/>
+      <c r="C80" s="86"/>
+      <c r="D80" s="86"/>
+      <c r="E80" s="86"/>
+      <c r="F80" s="86"/>
+      <c r="G80" s="86"/>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A81" s="99" t="s">
+        <v>4751</v>
+      </c>
+      <c r="B81" s="99"/>
+      <c r="C81" s="99">
+        <v>16</v>
+      </c>
+      <c r="D81" s="99" t="s">
+        <v>4665</v>
+      </c>
+      <c r="E81" s="99"/>
+      <c r="F81" s="99" t="s">
+        <v>4664</v>
+      </c>
+      <c r="G81" s="99" t="s">
+        <v>4666</v>
+      </c>
+      <c r="P81" s="100" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B82" s="99" t="s">
+        <v>4752</v>
+      </c>
+      <c r="G82" s="99" t="s">
+        <v>4667</v>
+      </c>
+      <c r="P82" s="99" t="s">
+        <v>2952</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B83" s="99" t="s">
+        <v>2536</v>
+      </c>
+      <c r="G83" s="99" t="s">
+        <v>4668</v>
+      </c>
+      <c r="P83" s="99" t="s">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B84" s="99" t="s">
+        <v>4756</v>
+      </c>
+      <c r="G84" s="99"/>
+      <c r="P84" s="99" t="s">
+        <v>4769</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B85" s="99" t="s">
+        <v>4757</v>
+      </c>
+      <c r="G85" s="99"/>
+      <c r="P85" s="99" t="s">
+        <v>4770</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B86" s="99" t="s">
+        <v>2921</v>
+      </c>
+      <c r="G86" s="99"/>
+      <c r="P86" s="99" t="s">
+        <v>2921</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B87" s="99" t="s">
+        <v>4758</v>
+      </c>
+      <c r="G87" s="99"/>
+      <c r="P87" s="99" t="s">
+        <v>4760</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B88" s="99" t="s">
+        <v>4759</v>
+      </c>
+      <c r="G88" s="99"/>
+      <c r="P88" s="99" t="s">
+        <v>4761</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B89" s="99" t="s">
+        <v>4735</v>
+      </c>
+      <c r="G89" s="99"/>
+      <c r="P89" s="99" t="s">
+        <v>4742</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A90" s="86"/>
+      <c r="B90" s="86"/>
+      <c r="C90" s="86"/>
+      <c r="D90" s="86"/>
+      <c r="E90" s="86"/>
+      <c r="F90" s="86"/>
+      <c r="G90" s="86"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A91" s="98" t="s">
+        <v>4771</v>
+      </c>
+      <c r="B91" s="98"/>
+      <c r="C91" s="98">
+        <v>17</v>
+      </c>
+      <c r="D91" s="98" t="s">
+        <v>4659</v>
+      </c>
+      <c r="E91" s="98"/>
+      <c r="F91" s="98" t="s">
+        <v>4657</v>
+      </c>
+      <c r="G91" s="98" t="s">
+        <v>4661</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G92" s="98" t="s">
+        <v>4662</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A94" s="98" t="s">
+        <v>4777</v>
+      </c>
+      <c r="B94" s="98"/>
+      <c r="C94" s="98">
+        <v>18</v>
+      </c>
+      <c r="D94" s="98" t="s">
+        <v>4674</v>
+      </c>
+      <c r="E94" s="98"/>
+      <c r="F94" s="98" t="s">
+        <v>4672</v>
+      </c>
+      <c r="G94" s="98" t="s">
+        <v>4676</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A98" s="87" t="s">
+        <v>4778</v>
+      </c>
+      <c r="B98" s="87"/>
+      <c r="C98" s="87">
+        <v>19</v>
+      </c>
+      <c r="D98" s="87" t="s">
+        <v>4679</v>
+      </c>
+      <c r="E98" s="87"/>
+      <c r="F98" s="87" t="s">
+        <v>4678</v>
+      </c>
+      <c r="G98" s="87" t="s">
+        <v>4680</v>
+      </c>
+      <c r="Q98" s="100" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B99" s="87" t="s">
+        <v>4687</v>
+      </c>
+      <c r="G99" s="87" t="s">
+        <v>4681</v>
+      </c>
+      <c r="Q99" s="87" t="s">
+        <v>2961</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B100" s="87" t="s">
+        <v>4772</v>
+      </c>
+      <c r="Q100" s="87" t="s">
+        <v>2952</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B101" s="87" t="s">
+        <v>4736</v>
+      </c>
+      <c r="Q101" s="87" t="s">
+        <v>4743</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B102" s="87" t="s">
+        <v>4773</v>
+      </c>
+      <c r="Q102" s="87" t="s">
+        <v>4779</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B103" s="87" t="s">
+        <v>4774</v>
+      </c>
+      <c r="Q103" s="87" t="s">
+        <v>4780</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B104" s="87" t="s">
+        <v>4775</v>
+      </c>
+      <c r="Q104" s="87" t="s">
+        <v>4781</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B105" s="87" t="s">
+        <v>4776</v>
+      </c>
+      <c r="Q105" s="87" t="s">
+        <v>4782</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A107" s="98" t="s">
+        <v>4783</v>
+      </c>
+      <c r="B107" s="98"/>
+      <c r="C107" s="98">
+        <v>20</v>
+      </c>
+      <c r="D107" s="98" t="s">
+        <v>4675</v>
+      </c>
+      <c r="E107" s="98"/>
+      <c r="F107" s="98" t="s">
+        <v>4673</v>
+      </c>
+      <c r="G107" s="98" t="s">
+        <v>4677</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="contents!A1" display="Contents" xr:uid="{130BE287-3EA5-4EB6-8CF1-366FB5569012}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
@@ -34607,7 +36502,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
@@ -35217,7 +37112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE91EB1-743A-4EB0-8CA9-D92D8C0FFFD2}">
   <dimension ref="A1:L17"/>
   <sheetViews>
@@ -35372,7 +37267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:J106"/>
   <sheetViews>
@@ -37519,7 +39414,684 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D4" t="s">
+        <v>307</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D5" t="s">
+        <v>309</v>
+      </c>
+      <c r="E5">
+        <v>60</v>
+      </c>
+      <c r="F5">
+        <v>60</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D6" t="s">
+        <v>312</v>
+      </c>
+      <c r="E6">
+        <v>90</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D7" t="s">
+        <v>313</v>
+      </c>
+      <c r="E7">
+        <v>90</v>
+      </c>
+      <c r="F7">
+        <v>40</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D8" t="s">
+        <v>313</v>
+      </c>
+      <c r="E8">
+        <v>90</v>
+      </c>
+      <c r="F8">
+        <v>40</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D9" t="s">
+        <v>317</v>
+      </c>
+      <c r="E9">
+        <v>120</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D10" t="s">
+        <v>318</v>
+      </c>
+      <c r="E10">
+        <v>90</v>
+      </c>
+      <c r="F10">
+        <v>40</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D11" t="s">
+        <v>320</v>
+      </c>
+      <c r="E11">
+        <v>120</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D12" t="s">
+        <v>317</v>
+      </c>
+      <c r="E12">
+        <v>120</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D13" t="s">
+        <v>320</v>
+      </c>
+      <c r="E13">
+        <v>120</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D14" t="s">
+        <v>323</v>
+      </c>
+      <c r="E14">
+        <v>120</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D15" t="s">
+        <v>325</v>
+      </c>
+      <c r="E15">
+        <v>120</v>
+      </c>
+      <c r="F15">
+        <v>20</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D16" t="s">
+        <v>327</v>
+      </c>
+      <c r="E16">
+        <v>90</v>
+      </c>
+      <c r="F16">
+        <v>40</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D17" t="s">
+        <v>329</v>
+      </c>
+      <c r="E17">
+        <v>90</v>
+      </c>
+      <c r="F17">
+        <v>40</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D18" t="s">
+        <v>331</v>
+      </c>
+      <c r="E18">
+        <v>90</v>
+      </c>
+      <c r="F18">
+        <v>40</v>
+      </c>
+      <c r="G18">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>333</v>
+      </c>
+      <c r="D19" t="s">
+        <v>333</v>
+      </c>
+      <c r="E19">
+        <v>30</v>
+      </c>
+      <c r="F19">
+        <v>25</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>333</v>
+      </c>
+      <c r="D20" t="s">
+        <v>335</v>
+      </c>
+      <c r="E20">
+        <v>30</v>
+      </c>
+      <c r="F20">
+        <v>25</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D21" t="s">
+        <v>338</v>
+      </c>
+      <c r="E21">
+        <v>160</v>
+      </c>
+      <c r="F21">
+        <v>30</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D22" t="s">
+        <v>340</v>
+      </c>
+      <c r="E22">
+        <v>160</v>
+      </c>
+      <c r="F22">
+        <v>30</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D23" t="s">
+        <v>340</v>
+      </c>
+      <c r="E23">
+        <v>160</v>
+      </c>
+      <c r="F23">
+        <v>30</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D24" t="s">
+        <v>338</v>
+      </c>
+      <c r="E24">
+        <v>160</v>
+      </c>
+      <c r="F24">
+        <v>30</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="contents!A1" display="Contents" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:CK198"/>
   <sheetViews>
@@ -47601,684 +50173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I24"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="D4" t="s">
-        <v>307</v>
-      </c>
-      <c r="E4">
-        <v>60</v>
-      </c>
-      <c r="F4">
-        <v>60</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>12</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="D5" t="s">
-        <v>309</v>
-      </c>
-      <c r="E5">
-        <v>60</v>
-      </c>
-      <c r="F5">
-        <v>60</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>12</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D6" t="s">
-        <v>312</v>
-      </c>
-      <c r="E6">
-        <v>90</v>
-      </c>
-      <c r="F6">
-        <v>40</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D7" t="s">
-        <v>313</v>
-      </c>
-      <c r="E7">
-        <v>90</v>
-      </c>
-      <c r="F7">
-        <v>40</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D8" t="s">
-        <v>313</v>
-      </c>
-      <c r="E8">
-        <v>90</v>
-      </c>
-      <c r="F8">
-        <v>40</v>
-      </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="D9" t="s">
-        <v>317</v>
-      </c>
-      <c r="E9">
-        <v>120</v>
-      </c>
-      <c r="F9">
-        <v>20</v>
-      </c>
-      <c r="G9">
-        <v>7</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D10" t="s">
-        <v>318</v>
-      </c>
-      <c r="E10">
-        <v>90</v>
-      </c>
-      <c r="F10">
-        <v>40</v>
-      </c>
-      <c r="G10">
-        <v>10</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="D11" t="s">
-        <v>320</v>
-      </c>
-      <c r="E11">
-        <v>120</v>
-      </c>
-      <c r="F11">
-        <v>20</v>
-      </c>
-      <c r="G11">
-        <v>7</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="D12" t="s">
-        <v>317</v>
-      </c>
-      <c r="E12">
-        <v>120</v>
-      </c>
-      <c r="F12">
-        <v>20</v>
-      </c>
-      <c r="G12">
-        <v>7</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="D13" t="s">
-        <v>320</v>
-      </c>
-      <c r="E13">
-        <v>120</v>
-      </c>
-      <c r="F13">
-        <v>20</v>
-      </c>
-      <c r="G13">
-        <v>7</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="D14" t="s">
-        <v>323</v>
-      </c>
-      <c r="E14">
-        <v>120</v>
-      </c>
-      <c r="F14">
-        <v>20</v>
-      </c>
-      <c r="G14">
-        <v>7</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="D15" t="s">
-        <v>325</v>
-      </c>
-      <c r="E15">
-        <v>120</v>
-      </c>
-      <c r="F15">
-        <v>20</v>
-      </c>
-      <c r="G15">
-        <v>7</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D16" t="s">
-        <v>327</v>
-      </c>
-      <c r="E16">
-        <v>90</v>
-      </c>
-      <c r="F16">
-        <v>40</v>
-      </c>
-      <c r="G16">
-        <v>10</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D17" t="s">
-        <v>329</v>
-      </c>
-      <c r="E17">
-        <v>90</v>
-      </c>
-      <c r="F17">
-        <v>40</v>
-      </c>
-      <c r="G17">
-        <v>10</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D18" t="s">
-        <v>331</v>
-      </c>
-      <c r="E18">
-        <v>90</v>
-      </c>
-      <c r="F18">
-        <v>40</v>
-      </c>
-      <c r="G18">
-        <v>10</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>333</v>
-      </c>
-      <c r="D19" t="s">
-        <v>333</v>
-      </c>
-      <c r="E19">
-        <v>30</v>
-      </c>
-      <c r="F19">
-        <v>25</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>333</v>
-      </c>
-      <c r="D20" t="s">
-        <v>335</v>
-      </c>
-      <c r="E20">
-        <v>30</v>
-      </c>
-      <c r="F20">
-        <v>25</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="D21" t="s">
-        <v>338</v>
-      </c>
-      <c r="E21">
-        <v>160</v>
-      </c>
-      <c r="F21">
-        <v>30</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="D22" t="s">
-        <v>340</v>
-      </c>
-      <c r="E22">
-        <v>160</v>
-      </c>
-      <c r="F22">
-        <v>30</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="D23" t="s">
-        <v>340</v>
-      </c>
-      <c r="E23">
-        <v>160</v>
-      </c>
-      <c r="F23">
-        <v>30</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="D24" t="s">
-        <v>338</v>
-      </c>
-      <c r="E24">
-        <v>160</v>
-      </c>
-      <c r="F24">
-        <v>30</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" location="contents!A1" display="Contents" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A3:J106"/>
   <sheetViews>
@@ -50099,7 +51994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
@@ -50264,7 +52159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:A121"/>
   <sheetViews>
@@ -57927,57 +59822,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1140:A1048576 A3:A8 A64:A115 A171:A177 A198:A208 A211:A214 A43:A61 A10:A17 A179:A196 A216:A229 A19:A41">
-    <cfRule type="duplicateValues" dxfId="26" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A197">
-    <cfRule type="duplicateValues" dxfId="25" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144:A155 A170">
-    <cfRule type="duplicateValues" dxfId="24" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A116:A123 A125:A128">
-    <cfRule type="duplicateValues" dxfId="23" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A116:A123 A125:A128">
-    <cfRule type="duplicateValues" dxfId="22" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A156:A161 A166:A169">
-    <cfRule type="duplicateValues" dxfId="20" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="duplicateValues" dxfId="19" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A474:A1048576 A327:A329 A3:A8 A210:A214 A43:A115 A171:A208 A216:A282 A162:A165 E124 A10:A41 A286:A319">
-    <cfRule type="duplicateValues" dxfId="18" priority="32"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A474:A1048576 A327:A329 A3:A8 A43:A115 A129:A143 A171:A282 A162:A165 E124 A10:A41 A286:A319">
-    <cfRule type="duplicateValues" dxfId="16" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A474:A1048576 A326:A331 A162:A165 E124 A125:A155 A3:A123 A170:A323">
-    <cfRule type="duplicateValues" dxfId="15" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A474:A1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A474:A1048576 A326:A331 A3:A323">
-    <cfRule type="duplicateValues" dxfId="13" priority="38"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A332:A447">
-    <cfRule type="duplicateValues" dxfId="11" priority="96"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="97"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="96"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A332:A447">
-    <cfRule type="duplicateValues" dxfId="9" priority="100"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A448:A473">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A448:A473">
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="contents!A1" display="Contents" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
@@ -59086,7 +60981,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E3">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="contents!A1" display="Contents" xr:uid="{8EA37169-2323-40C3-9046-4C9A4C68151F}"/>
@@ -59109,9 +61004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S130"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>